<commit_message>
Big Update : - JP translate - Adding Raw Lineup winrates - Adding JCG Profile - Adding Player Wins - Reworking EM
</commit_message>
<xml_diff>
--- a/Excel_and_CSV/OmenMeta.xlsx
+++ b/Excel_and_CSV/OmenMeta.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24701"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24827"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Python_WS\Github_SV\Excel_and_CSV\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6CDC78AA-C319-452E-BDEF-2A65C988585F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{14CA4C6F-A795-4821-8141-3276AC992648}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20640" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="321" uniqueCount="180">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="449" uniqueCount="218">
   <si>
     <t>Archetype Name</t>
   </si>
@@ -80,15 +80,6 @@
     <t>Sword</t>
   </si>
   <si>
-    <t>Cat Admiral</t>
-  </si>
-  <si>
-    <t>7AfHi</t>
-  </si>
-  <si>
-    <t>Levin OTK Sword</t>
-  </si>
-  <si>
     <t>Albert, Thunderous Doom</t>
   </si>
   <si>
@@ -170,21 +161,12 @@
     <t>7BSYy</t>
   </si>
   <si>
-    <t>Natura Dragon</t>
-  </si>
-  <si>
     <t>Naterra's Future</t>
   </si>
   <si>
     <t>7DjKQ</t>
   </si>
   <si>
-    <t>Touching Thoughts</t>
-  </si>
-  <si>
-    <t>7FA5w</t>
-  </si>
-  <si>
     <t>Machina Shadow</t>
   </si>
   <si>
@@ -212,12 +194,6 @@
     <t>7BpFw</t>
   </si>
   <si>
-    <t>Ominous Tyrant</t>
-  </si>
-  <si>
-    <t>7Bqzc</t>
-  </si>
-  <si>
     <t>Blood</t>
   </si>
   <si>
@@ -287,24 +263,12 @@
     <t>7GoLy</t>
   </si>
   <si>
-    <t>Absolute Tolerance</t>
-  </si>
-  <si>
-    <t>7C-D6</t>
-  </si>
-  <si>
     <t>gcvky</t>
   </si>
   <si>
     <t>Artifact Portal</t>
   </si>
   <si>
-    <t>Artifact Carrier</t>
-  </si>
-  <si>
-    <t>7Cxmi</t>
-  </si>
-  <si>
     <t>Genesis Artifact</t>
   </si>
   <si>
@@ -362,212 +326,362 @@
     <t>7G1X6</t>
   </si>
   <si>
+    <t>Heavenly Help</t>
+  </si>
+  <si>
+    <t>7K9h2</t>
+  </si>
+  <si>
+    <t>78nfc</t>
+  </si>
+  <si>
+    <t>Frigg</t>
+  </si>
+  <si>
+    <t>Djeana, the Stouthearted</t>
+  </si>
+  <si>
+    <t>7FEFY</t>
+  </si>
+  <si>
+    <t>Suzy, Hexcaster</t>
+  </si>
+  <si>
+    <t>7JQpC</t>
+  </si>
+  <si>
+    <t>Cernunnos</t>
+  </si>
+  <si>
+    <t>7JTFc</t>
+  </si>
+  <si>
+    <t>Imagination Realized</t>
+  </si>
+  <si>
+    <t>7Igiw</t>
+  </si>
+  <si>
+    <t>Piercye, Queen of Frost</t>
+  </si>
+  <si>
+    <t>7Hsiy</t>
+  </si>
+  <si>
+    <t>7LlkS</t>
+  </si>
+  <si>
+    <t>Ladica Forest</t>
+  </si>
+  <si>
+    <t>Kagemitsu, Lost Samurai</t>
+  </si>
+  <si>
+    <t>7M88o</t>
+  </si>
+  <si>
+    <t>Monochrome Endgame</t>
+  </si>
+  <si>
+    <t>7IKkg</t>
+  </si>
+  <si>
+    <t>Acid Golem</t>
+  </si>
+  <si>
+    <t>7MU7C</t>
+  </si>
+  <si>
+    <t>Evo Rune</t>
+  </si>
+  <si>
+    <t>Burn Dragon</t>
+  </si>
+  <si>
+    <t>Rowen, Dragon Lance</t>
+  </si>
+  <si>
+    <t>7FGi6</t>
+  </si>
+  <si>
+    <t>Evo Blood</t>
+  </si>
+  <si>
+    <t>Yuzuki, Bloodlord</t>
+  </si>
+  <si>
+    <t>7Nfoo</t>
+  </si>
+  <si>
+    <t>Amulet Haven</t>
+  </si>
+  <si>
+    <t>7KE4I</t>
+  </si>
+  <si>
+    <t>God of Curses</t>
+  </si>
+  <si>
+    <t>Wilbert, Luminous Paladin</t>
+  </si>
+  <si>
+    <t>7O2DI</t>
+  </si>
+  <si>
+    <t>Frigg Haven</t>
+  </si>
+  <si>
+    <t>Heal Haven</t>
+  </si>
+  <si>
+    <t>Bellerophon</t>
+  </si>
+  <si>
+    <t>7O2DS</t>
+  </si>
+  <si>
+    <t>Evo Haven</t>
+  </si>
+  <si>
+    <t>Evo Portal</t>
+  </si>
+  <si>
+    <t>Aggro Portal</t>
+  </si>
+  <si>
+    <t>Colossus Omega</t>
+  </si>
+  <si>
+    <t>79A46</t>
+  </si>
+  <si>
+    <t>Jetpack OTK Portal</t>
+  </si>
+  <si>
+    <t>Managrocer</t>
+  </si>
+  <si>
+    <t>79s0I</t>
+  </si>
+  <si>
+    <t>Jetpack Gunner</t>
+  </si>
+  <si>
+    <t>7OOBi</t>
+  </si>
+  <si>
+    <t>Roy, Dragonreaver</t>
+  </si>
+  <si>
+    <t>7BQ6Y</t>
+  </si>
+  <si>
+    <t>Muskfruit</t>
+  </si>
+  <si>
+    <t>7GN-I</t>
+  </si>
+  <si>
+    <t>Sacred Ice-Crusher</t>
+  </si>
+  <si>
+    <t>7NzKy</t>
+  </si>
+  <si>
+    <t>Calamity Portal</t>
+  </si>
+  <si>
+    <t>Calamity's Genesis</t>
+  </si>
+  <si>
+    <t>7KdDg</t>
+  </si>
+  <si>
+    <t>Bloodlust Demon</t>
+  </si>
+  <si>
+    <t>7Jrg6</t>
+  </si>
+  <si>
+    <t>Hybrid Forest</t>
+  </si>
+  <si>
+    <t>Leod Sword</t>
+  </si>
+  <si>
+    <t>Auction the Spoils</t>
+  </si>
+  <si>
+    <t>7AdaA</t>
+  </si>
+  <si>
+    <t>Linkstaff Necromancer</t>
+  </si>
+  <si>
+    <t>7FXnY</t>
+  </si>
+  <si>
+    <t>Control Forest</t>
+  </si>
+  <si>
+    <t>Izudia, Unkilling Annihilation</t>
+  </si>
+  <si>
+    <t>Kuon, Wuxing Master</t>
+  </si>
+  <si>
+    <t>7MWZI</t>
+  </si>
+  <si>
+    <t>OTK Shadow</t>
+  </si>
+  <si>
+    <t>Ceres, Bride of the Night</t>
+  </si>
+  <si>
+    <t>7BqzI</t>
+  </si>
+  <si>
+    <t>7FaDy</t>
+  </si>
+  <si>
+    <t>Flame Zombie</t>
+  </si>
+  <si>
+    <t>Mobilized Factory</t>
+  </si>
+  <si>
+    <t>797di</t>
+  </si>
+  <si>
+    <t>Lishenna Portal</t>
+  </si>
+  <si>
+    <t>Lishenna, Melodious Destruction</t>
+  </si>
+  <si>
+    <t>7OQe6</t>
+  </si>
+  <si>
+    <t>OTK Sword</t>
+  </si>
+  <si>
+    <t>Eahta, God of the Blade</t>
+  </si>
+  <si>
+    <t>76tao</t>
+  </si>
+  <si>
+    <t>Jerry Dragon</t>
+  </si>
+  <si>
+    <t>Mjerrabaine, Great One</t>
+  </si>
+  <si>
+    <t>7LNJo</t>
+  </si>
+  <si>
+    <t>Jerry Sword</t>
+  </si>
+  <si>
+    <t>Midrange Sword</t>
+  </si>
+  <si>
+    <t>Leod, the Crescent Blade</t>
+  </si>
+  <si>
+    <t>6eK0Y</t>
+  </si>
+  <si>
+    <t>Frenzied Corpsmaster</t>
+  </si>
+  <si>
+    <t>7ETQY</t>
+  </si>
+  <si>
+    <t>Jerry Blood</t>
+  </si>
+  <si>
+    <t>7Nfoy</t>
+  </si>
+  <si>
+    <t>Pain Immortal</t>
+  </si>
+  <si>
+    <t>Rulenye Shadow</t>
+  </si>
+  <si>
+    <t>Rulenye, Screaming Silence</t>
+  </si>
+  <si>
+    <t>7NHOc</t>
+  </si>
+  <si>
+    <t>Adherent of Screams</t>
+  </si>
+  <si>
+    <t>7NCW6</t>
+  </si>
+  <si>
+    <t>Natura Burn Dragon</t>
+  </si>
+  <si>
+    <t>Brutal Dragonewt</t>
+  </si>
+  <si>
+    <t>7J4r6</t>
+  </si>
+  <si>
+    <t>Jerry Portal</t>
+  </si>
+  <si>
+    <t>Jerry Haven</t>
+  </si>
+  <si>
+    <t>Jerry Shadow</t>
+  </si>
+  <si>
+    <t>7JTFI</t>
+  </si>
+  <si>
+    <t>Skeleton Raider</t>
+  </si>
+  <si>
+    <t>Jerry Rune</t>
+  </si>
+  <si>
+    <t>Banesbow Elf</t>
+  </si>
+  <si>
+    <t>7Lgry</t>
+  </si>
+  <si>
+    <t>Kagero, Swordbound Soul</t>
+  </si>
+  <si>
+    <t>7BqzS</t>
+  </si>
+  <si>
+    <t>Jerry Forest</t>
+  </si>
+  <si>
     <t>Aggro Rally Sword</t>
   </si>
   <si>
-    <t>Evo Rally Sword</t>
-  </si>
-  <si>
-    <t>Heavenly Help</t>
-  </si>
-  <si>
-    <t>7K9h2</t>
-  </si>
-  <si>
-    <t>78nfc</t>
-  </si>
-  <si>
-    <t>Frigg</t>
-  </si>
-  <si>
-    <t>Djeana, the Stouthearted</t>
-  </si>
-  <si>
-    <t>7FEFY</t>
-  </si>
-  <si>
-    <t>Erika, Loyal Swordsavant</t>
-  </si>
-  <si>
-    <t>7EVt6</t>
-  </si>
-  <si>
-    <t>Suzy, Hexcaster</t>
-  </si>
-  <si>
-    <t>7JQpC</t>
-  </si>
-  <si>
-    <t>Cernunnos</t>
-  </si>
-  <si>
-    <t>7JTFc</t>
-  </si>
-  <si>
-    <t>Imagination Realized</t>
-  </si>
-  <si>
-    <t>7Igiw</t>
-  </si>
-  <si>
-    <t>Piercye, Queen of Frost</t>
-  </si>
-  <si>
-    <t>Breezy Elf</t>
-  </si>
-  <si>
-    <t>7Hsiy</t>
-  </si>
-  <si>
-    <t>7LlkS</t>
-  </si>
-  <si>
-    <t>Ladica Forest</t>
-  </si>
-  <si>
-    <t>Kagemitsu, Lost Samurai</t>
-  </si>
-  <si>
-    <t>7M88o</t>
-  </si>
-  <si>
-    <t>Monochrome Endgame</t>
-  </si>
-  <si>
-    <t>7IKkg</t>
-  </si>
-  <si>
-    <t>Coronation Sword</t>
-  </si>
-  <si>
-    <t>Coronation</t>
-  </si>
-  <si>
-    <t>7IIIQ</t>
-  </si>
-  <si>
-    <t>7EVsy</t>
-  </si>
-  <si>
-    <t>Leod, Moonlit Executioner</t>
-  </si>
-  <si>
-    <t>Evo Forest</t>
-  </si>
-  <si>
-    <t>Acid Golem</t>
-  </si>
-  <si>
-    <t>7MU7C</t>
-  </si>
-  <si>
-    <t>Evo Rune</t>
-  </si>
-  <si>
-    <t>Evo Dragon</t>
-  </si>
-  <si>
-    <t>Burn Dragon</t>
-  </si>
-  <si>
-    <t>Rowen, Dragon Lance</t>
-  </si>
-  <si>
-    <t>7FGi6</t>
+    <t>Penguin Guardian</t>
+  </si>
+  <si>
+    <t>7M0qM</t>
   </si>
   <si>
     <t>Evo Shadow</t>
-  </si>
-  <si>
-    <t>Evo Blood</t>
-  </si>
-  <si>
-    <t>Yuzuki, Bloodlord</t>
-  </si>
-  <si>
-    <t>7Nfoo</t>
-  </si>
-  <si>
-    <t>Amulet Haven</t>
-  </si>
-  <si>
-    <t>7KE4I</t>
-  </si>
-  <si>
-    <t>God of Curses</t>
-  </si>
-  <si>
-    <t>Wilbert, Luminous Paladin</t>
-  </si>
-  <si>
-    <t>7O2DI</t>
-  </si>
-  <si>
-    <t>Frigg Haven</t>
-  </si>
-  <si>
-    <t>Heal Haven</t>
-  </si>
-  <si>
-    <t>Bellerophon</t>
-  </si>
-  <si>
-    <t>7O2DS</t>
-  </si>
-  <si>
-    <t>Evo Haven</t>
-  </si>
-  <si>
-    <t>Evo Portal</t>
-  </si>
-  <si>
-    <t>Aggro Portal</t>
-  </si>
-  <si>
-    <t>Colossus Omega</t>
-  </si>
-  <si>
-    <t>79A46</t>
-  </si>
-  <si>
-    <t>Jetpack OTK Portal</t>
-  </si>
-  <si>
-    <t>Managrocer</t>
-  </si>
-  <si>
-    <t>79s0I</t>
-  </si>
-  <si>
-    <t>Jetpack Gunner</t>
-  </si>
-  <si>
-    <t>7OOBi</t>
-  </si>
-  <si>
-    <t>Roy, Dragonreaver</t>
-  </si>
-  <si>
-    <t>7BQ6Y</t>
-  </si>
-  <si>
-    <t>Muskfruit</t>
-  </si>
-  <si>
-    <t>7GN-I</t>
-  </si>
-  <si>
-    <t>Sacred Ice-Crusher</t>
-  </si>
-  <si>
-    <t>7NzKy</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="7" x14ac:knownFonts="1">
+  <fonts count="8" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
       <color rgb="FF000000"/>
@@ -611,6 +725,13 @@
       <name val="Arial"/>
       <family val="2"/>
     </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -632,7 +753,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
@@ -642,6 +763,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -860,10 +982,10 @@
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
-  <dimension ref="A1:I1000"/>
+  <dimension ref="A1:I1015"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A16" workbookViewId="0">
-      <selection activeCell="F33" sqref="F33"/>
+    <sheetView tabSelected="1" topLeftCell="A22" workbookViewId="0">
+      <selection activeCell="E38" sqref="E38"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -889,40 +1011,40 @@
         <v>2</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>104</v>
+        <v>92</v>
       </c>
       <c r="E1" s="1" t="s">
         <v>3</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>105</v>
+        <v>93</v>
       </c>
       <c r="G1" s="1" t="s">
         <v>4</v>
       </c>
       <c r="H1" s="1" t="s">
-        <v>106</v>
+        <v>94</v>
       </c>
       <c r="I1" s="2"/>
     </row>
-    <row r="2" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:9" s="6" customFormat="1" ht="15" x14ac:dyDescent="0.25">
       <c r="A2" s="3" t="s">
-        <v>143</v>
+        <v>213</v>
       </c>
       <c r="B2" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="C2" s="4" t="s">
-        <v>129</v>
-      </c>
-      <c r="D2" s="4" t="s">
-        <v>132</v>
-      </c>
-      <c r="E2" s="4" t="s">
-        <v>130</v>
-      </c>
-      <c r="F2" s="4" t="s">
-        <v>131</v>
+      <c r="C2" s="3" t="s">
+        <v>184</v>
+      </c>
+      <c r="D2" s="3" t="s">
+        <v>185</v>
+      </c>
+      <c r="E2" s="1" t="s">
+        <v>209</v>
+      </c>
+      <c r="F2" s="1" t="s">
+        <v>210</v>
       </c>
       <c r="G2" s="4" t="s">
         <v>6</v>
@@ -930,1120 +1052,1492 @@
       <c r="H2" s="4" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="3" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="I2" s="2"/>
+    </row>
+    <row r="3" spans="1:9" s="6" customFormat="1" ht="15" x14ac:dyDescent="0.25">
       <c r="A3" s="3" t="s">
-        <v>133</v>
+        <v>166</v>
       </c>
       <c r="B3" s="3" t="s">
         <v>5</v>
       </c>
       <c r="C3" s="4" t="s">
-        <v>7</v>
+        <v>113</v>
       </c>
       <c r="D3" s="4" t="s">
-        <v>8</v>
+        <v>115</v>
       </c>
       <c r="E3" s="4" t="s">
-        <v>9</v>
+        <v>167</v>
       </c>
       <c r="F3" s="4" t="s">
-        <v>10</v>
+        <v>114</v>
       </c>
       <c r="G3" s="4" t="s">
-        <v>6</v>
-      </c>
-      <c r="H3" s="3" t="s">
-        <v>6</v>
-      </c>
+        <v>12</v>
+      </c>
+      <c r="H3" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="I3" s="2"/>
     </row>
     <row r="4" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="3" t="s">
-        <v>11</v>
+        <v>166</v>
       </c>
       <c r="B4" s="3" t="s">
         <v>5</v>
       </c>
       <c r="C4" s="4" t="s">
+        <v>113</v>
+      </c>
+      <c r="D4" s="4" t="s">
+        <v>115</v>
+      </c>
+      <c r="E4" s="4" t="s">
+        <v>167</v>
+      </c>
+      <c r="F4" s="4" t="s">
+        <v>114</v>
+      </c>
+      <c r="G4" s="4" t="s">
         <v>12</v>
       </c>
-      <c r="D4" s="4" t="s">
+      <c r="H4" s="4" t="s">
         <v>13</v>
       </c>
-      <c r="E4" s="4" t="s">
-        <v>14</v>
-      </c>
-      <c r="F4" s="4" t="s">
-        <v>15</v>
-      </c>
-      <c r="G4" s="4" t="s">
-        <v>7</v>
-      </c>
-      <c r="H4" s="4" t="s">
-        <v>8</v>
-      </c>
     </row>
     <row r="5" spans="1:9" s="6" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="5" t="s">
-        <v>11</v>
+      <c r="A5" s="3" t="s">
+        <v>160</v>
       </c>
       <c r="B5" s="3" t="s">
         <v>5</v>
       </c>
       <c r="C5" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="D5" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="E5" s="4" t="s">
         <v>12</v>
       </c>
-      <c r="D5" s="4" t="s">
-        <v>16</v>
-      </c>
-      <c r="E5" s="4" t="s">
-        <v>14</v>
-      </c>
       <c r="F5" s="4" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="G5" s="4" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="H5" s="4" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
     </row>
     <row r="6" spans="1:9" s="6" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="3" t="s">
-        <v>17</v>
+        <v>160</v>
       </c>
       <c r="B6" s="3" t="s">
         <v>5</v>
       </c>
       <c r="C6" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="D6" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="E6" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="F6" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="G6" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="H6" s="4" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="7" spans="1:9" s="6" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A7" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="B7" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="C7" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="D7" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="E7" s="4" t="s">
         <v>14</v>
       </c>
-      <c r="D6" s="4" t="s">
+      <c r="F7" s="4" t="s">
         <v>15</v>
       </c>
-      <c r="E6" s="4" t="s">
+      <c r="G7" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="H7" s="4" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="8" spans="1:9" s="6" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A8" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="B8" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="C8" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="D8" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="E8" s="4" t="s">
         <v>14</v>
       </c>
-      <c r="F6" s="4" t="s">
+      <c r="F8" s="4" t="s">
         <v>15</v>
       </c>
-      <c r="G6" s="3" t="s">
-        <v>6</v>
-      </c>
-      <c r="H6" s="3" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="7" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="4" t="s">
+      <c r="G8" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="H8" s="4" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="9" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A9" s="3" t="s">
+        <v>116</v>
+      </c>
+      <c r="B9" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="C9" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="D9" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="E9" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="F9" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="G9" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="H9" s="3" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="10" spans="1:9" s="6" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A10" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="B10" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="C10" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="D10" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="E10" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="F10" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="G10" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="H10" s="3" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="11" spans="1:9" s="6" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A11" s="3" t="s">
+        <v>186</v>
+      </c>
+      <c r="B11" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="C11" s="3" t="s">
+        <v>184</v>
+      </c>
+      <c r="D11" s="3" t="s">
+        <v>185</v>
+      </c>
+      <c r="E11" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="F11" s="4" t="s">
+        <v>20</v>
+      </c>
+      <c r="G11" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="H11" s="3" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="12" spans="1:9" s="6" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A12" s="3" t="s">
+        <v>180</v>
+      </c>
+      <c r="B12" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="C12" s="9" t="s">
+        <v>181</v>
+      </c>
+      <c r="D12" s="4" t="s">
+        <v>182</v>
+      </c>
+      <c r="E12" s="4" t="s">
         <v>21</v>
       </c>
-      <c r="B7" s="3" t="s">
+      <c r="F12" s="4" t="s">
+        <v>22</v>
+      </c>
+      <c r="G12" s="3" t="s">
+        <v>117</v>
+      </c>
+      <c r="H12" s="3" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="13" spans="1:9" s="6" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A13" s="3" t="s">
+        <v>161</v>
+      </c>
+      <c r="B13" s="3" t="s">
         <v>18</v>
       </c>
-      <c r="C7" s="4" t="s">
-        <v>22</v>
-      </c>
-      <c r="D7" s="4" t="s">
+      <c r="C13" s="9" t="s">
+        <v>188</v>
+      </c>
+      <c r="D13" s="4" t="s">
+        <v>189</v>
+      </c>
+      <c r="E13" s="4" t="s">
+        <v>162</v>
+      </c>
+      <c r="F13" s="4" t="s">
+        <v>163</v>
+      </c>
+      <c r="G13" s="3" t="s">
+        <v>190</v>
+      </c>
+      <c r="H13" s="3" t="s">
+        <v>191</v>
+      </c>
+    </row>
+    <row r="14" spans="1:9" s="6" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A14" s="3" t="s">
+        <v>214</v>
+      </c>
+      <c r="B14" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="C14" s="9" t="s">
+        <v>215</v>
+      </c>
+      <c r="D14" s="4" t="s">
+        <v>216</v>
+      </c>
+      <c r="E14" s="3" t="s">
+        <v>190</v>
+      </c>
+      <c r="F14" s="3" t="s">
+        <v>191</v>
+      </c>
+      <c r="G14" s="3" t="s">
+        <v>117</v>
+      </c>
+      <c r="H14" s="3" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="15" spans="1:9" s="6" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A15" s="3" t="s">
+        <v>187</v>
+      </c>
+      <c r="B15" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="C15" s="3" t="s">
+        <v>190</v>
+      </c>
+      <c r="D15" s="3" t="s">
+        <v>191</v>
+      </c>
+      <c r="E15" s="3" t="s">
+        <v>190</v>
+      </c>
+      <c r="F15" s="3" t="s">
+        <v>191</v>
+      </c>
+      <c r="G15" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="H15" s="3" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="16" spans="1:9" s="6" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A16" s="3" t="s">
+        <v>187</v>
+      </c>
+      <c r="B16" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="C16" s="9" t="s">
+        <v>119</v>
+      </c>
+      <c r="D16" s="4" t="s">
+        <v>120</v>
+      </c>
+      <c r="E16" s="9" t="s">
+        <v>119</v>
+      </c>
+      <c r="F16" s="4" t="s">
+        <v>120</v>
+      </c>
+      <c r="G16" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="H16" s="3" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="17" spans="1:8" s="6" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A17" s="3" t="s">
+        <v>208</v>
+      </c>
+      <c r="B17" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="C17" s="3" t="s">
+        <v>184</v>
+      </c>
+      <c r="D17" s="3" t="s">
+        <v>185</v>
+      </c>
+      <c r="E17" s="3" t="s">
+        <v>37</v>
+      </c>
+      <c r="F17" s="3" t="s">
+        <v>38</v>
+      </c>
+      <c r="G17" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="H17" s="3" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="18" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A18" s="3" t="s">
         <v>23</v>
       </c>
-      <c r="E7" s="4" t="s">
+      <c r="B18" s="3" t="s">
         <v>24</v>
       </c>
-      <c r="F7" s="4" t="s">
+      <c r="C18" s="3" t="s">
         <v>25</v>
       </c>
-      <c r="G7" s="3" t="s">
-        <v>19</v>
-      </c>
-      <c r="H7" s="3" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="8" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A8" s="3" t="s">
-        <v>114</v>
-      </c>
-      <c r="B8" s="3" t="s">
-        <v>18</v>
-      </c>
-      <c r="C8" s="3" t="s">
+      <c r="D18" s="3" t="s">
+        <v>26</v>
+      </c>
+      <c r="E18" s="3" t="s">
+        <v>111</v>
+      </c>
+      <c r="F18" s="3" t="s">
+        <v>112</v>
+      </c>
+      <c r="G18" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="H18" s="4" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="19" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A19" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="B19" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="C19" s="3" t="s">
+        <v>28</v>
+      </c>
+      <c r="D19" s="3" t="s">
+        <v>29</v>
+      </c>
+      <c r="E19" s="3" t="s">
+        <v>30</v>
+      </c>
+      <c r="F19" s="3" t="s">
+        <v>31</v>
+      </c>
+      <c r="G19" s="3" t="s">
+        <v>32</v>
+      </c>
+      <c r="H19" s="3" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="20" spans="1:8" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="A20" s="3" t="s">
+        <v>36</v>
+      </c>
+      <c r="B20" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="C20" s="3" t="s">
+        <v>37</v>
+      </c>
+      <c r="D20" s="3" t="s">
+        <v>38</v>
+      </c>
+      <c r="E20" s="3" t="s">
+        <v>168</v>
+      </c>
+      <c r="F20" s="3" t="s">
+        <v>169</v>
+      </c>
+      <c r="G20" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="H20" s="3" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="21" spans="1:8" s="6" customFormat="1" ht="15" x14ac:dyDescent="0.25">
+      <c r="A21" s="4" t="s">
+        <v>39</v>
+      </c>
+      <c r="B21" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="C21" s="4" t="s">
+        <v>121</v>
+      </c>
+      <c r="D21" s="4" t="s">
+        <v>122</v>
+      </c>
+      <c r="E21" s="4" t="s">
+        <v>121</v>
+      </c>
+      <c r="F21" s="4" t="s">
+        <v>122</v>
+      </c>
+      <c r="G21" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="H21" s="3" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="22" spans="1:8" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="A22" s="3" t="s">
+        <v>123</v>
+      </c>
+      <c r="B22" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="C22" s="3" t="s">
+        <v>40</v>
+      </c>
+      <c r="D22" s="3" t="s">
+        <v>41</v>
+      </c>
+      <c r="E22" s="3" t="s">
+        <v>40</v>
+      </c>
+      <c r="F22" s="3" t="s">
+        <v>41</v>
+      </c>
+      <c r="G22" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="H22" s="3" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="23" spans="1:8" s="6" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="A23" s="3" t="s">
+        <v>183</v>
+      </c>
+      <c r="B23" s="3" t="s">
+        <v>43</v>
+      </c>
+      <c r="C23" s="3" t="s">
+        <v>184</v>
+      </c>
+      <c r="D23" s="3" t="s">
+        <v>185</v>
+      </c>
+      <c r="E23" s="3" t="s">
+        <v>201</v>
+      </c>
+      <c r="F23" s="3" t="s">
+        <v>202</v>
+      </c>
+      <c r="G23" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="H23" s="3" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="24" spans="1:8" s="6" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="A24" s="3" t="s">
+        <v>42</v>
+      </c>
+      <c r="B24" s="3" t="s">
+        <v>43</v>
+      </c>
+      <c r="C24" s="3" t="s">
+        <v>44</v>
+      </c>
+      <c r="D24" s="3" t="s">
+        <v>45</v>
+      </c>
+      <c r="E24" s="3" t="s">
+        <v>97</v>
+      </c>
+      <c r="F24" s="3" t="s">
+        <v>98</v>
+      </c>
+      <c r="G24" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="H24" s="3" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="25" spans="1:8" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="A25" s="3" t="s">
+        <v>124</v>
+      </c>
+      <c r="B25" s="3" t="s">
+        <v>43</v>
+      </c>
+      <c r="C25" s="3" t="s">
+        <v>125</v>
+      </c>
+      <c r="D25" s="3" t="s">
+        <v>126</v>
+      </c>
+      <c r="E25" s="3" t="s">
+        <v>149</v>
+      </c>
+      <c r="F25" s="3" t="s">
+        <v>150</v>
+      </c>
+      <c r="G25" s="3" t="s">
+        <v>46</v>
+      </c>
+      <c r="H25" s="3" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="26" spans="1:8" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="A26" s="3" t="s">
+        <v>200</v>
+      </c>
+      <c r="B26" s="3" t="s">
+        <v>43</v>
+      </c>
+      <c r="C26" s="3" t="s">
+        <v>46</v>
+      </c>
+      <c r="D26" s="3" t="s">
+        <v>47</v>
+      </c>
+      <c r="E26" s="3" t="s">
+        <v>105</v>
+      </c>
+      <c r="F26" s="3" t="s">
+        <v>106</v>
+      </c>
+      <c r="G26" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="H26" s="3" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="27" spans="1:8" s="6" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="A27" s="3" t="s">
+        <v>205</v>
+      </c>
+      <c r="B27" s="3" t="s">
+        <v>49</v>
+      </c>
+      <c r="C27" s="3" t="s">
+        <v>184</v>
+      </c>
+      <c r="D27" s="3" t="s">
+        <v>185</v>
+      </c>
+      <c r="E27" s="3" t="s">
+        <v>207</v>
+      </c>
+      <c r="F27" s="3" t="s">
+        <v>206</v>
+      </c>
+      <c r="G27" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="H27" s="3" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="28" spans="1:8" ht="15" x14ac:dyDescent="0.25">
+      <c r="A28" s="4" t="s">
+        <v>48</v>
+      </c>
+      <c r="B28" s="3" t="s">
+        <v>49</v>
+      </c>
+      <c r="C28" s="3" t="s">
+        <v>50</v>
+      </c>
+      <c r="D28" s="3" t="s">
+        <v>51</v>
+      </c>
+      <c r="E28" s="3" t="s">
+        <v>52</v>
+      </c>
+      <c r="F28" s="3" t="s">
+        <v>53</v>
+      </c>
+      <c r="G28" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="H28" s="3" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="29" spans="1:8" s="6" customFormat="1" ht="15" x14ac:dyDescent="0.25">
+      <c r="A29" s="4" t="s">
+        <v>170</v>
+      </c>
+      <c r="B29" s="3" t="s">
+        <v>49</v>
+      </c>
+      <c r="C29" s="3" t="s">
+        <v>171</v>
+      </c>
+      <c r="D29" s="3" t="s">
+        <v>172</v>
+      </c>
+      <c r="E29" s="3" t="s">
+        <v>174</v>
+      </c>
+      <c r="F29" s="3" t="s">
+        <v>173</v>
+      </c>
+      <c r="G29" s="4" t="s">
+        <v>164</v>
+      </c>
+      <c r="H29" s="4" t="s">
+        <v>165</v>
+      </c>
+    </row>
+    <row r="30" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A30" s="4" t="s">
+        <v>54</v>
+      </c>
+      <c r="B30" s="3" t="s">
+        <v>49</v>
+      </c>
+      <c r="C30" s="4" t="s">
+        <v>55</v>
+      </c>
+      <c r="D30" s="4" t="s">
+        <v>56</v>
+      </c>
+      <c r="E30" s="4" t="s">
+        <v>164</v>
+      </c>
+      <c r="F30" s="4" t="s">
+        <v>165</v>
+      </c>
+      <c r="G30" s="3" t="s">
+        <v>109</v>
+      </c>
+      <c r="H30" s="3" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="31" spans="1:8" ht="15" x14ac:dyDescent="0.25">
+      <c r="A31" s="4" t="s">
+        <v>217</v>
+      </c>
+      <c r="B31" s="3" t="s">
+        <v>49</v>
+      </c>
+      <c r="C31" s="3" t="s">
+        <v>107</v>
+      </c>
+      <c r="D31" s="3" t="s">
+        <v>108</v>
+      </c>
+      <c r="E31" s="3" t="s">
+        <v>109</v>
+      </c>
+      <c r="F31" s="3" t="s">
+        <v>110</v>
+      </c>
+      <c r="G31" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="H31" s="3" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="32" spans="1:8" s="6" customFormat="1" ht="15" x14ac:dyDescent="0.25">
+      <c r="A32" s="4" t="s">
+        <v>195</v>
+      </c>
+      <c r="B32" s="3" t="s">
+        <v>49</v>
+      </c>
+      <c r="C32" s="3" t="s">
+        <v>196</v>
+      </c>
+      <c r="D32" s="3" t="s">
+        <v>197</v>
+      </c>
+      <c r="E32" s="3" t="s">
+        <v>198</v>
+      </c>
+      <c r="F32" s="3" t="s">
+        <v>199</v>
+      </c>
+      <c r="G32" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="H32" s="3" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="33" spans="1:9" s="6" customFormat="1" ht="15" x14ac:dyDescent="0.25">
+      <c r="A33" s="4" t="s">
+        <v>54</v>
+      </c>
+      <c r="B33" s="3" t="s">
+        <v>49</v>
+      </c>
+      <c r="C33" s="4" t="s">
+        <v>55</v>
+      </c>
+      <c r="D33" s="4" t="s">
+        <v>56</v>
+      </c>
+      <c r="E33" s="3" t="s">
+        <v>211</v>
+      </c>
+      <c r="F33" s="3" t="s">
+        <v>212</v>
+      </c>
+      <c r="G33" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="H33" s="3" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="34" spans="1:9" s="6" customFormat="1" ht="15" x14ac:dyDescent="0.25">
+      <c r="A34" s="4" t="s">
+        <v>192</v>
+      </c>
+      <c r="B34" s="3" t="s">
+        <v>57</v>
+      </c>
+      <c r="C34" s="3" t="s">
+        <v>184</v>
+      </c>
+      <c r="D34" s="3" t="s">
+        <v>185</v>
+      </c>
+      <c r="E34" s="3" t="s">
+        <v>194</v>
+      </c>
+      <c r="F34" s="3" t="s">
+        <v>193</v>
+      </c>
+      <c r="G34" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="H34" s="3" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="35" spans="1:9" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="A35" s="3" t="s">
+        <v>58</v>
+      </c>
+      <c r="B35" s="3" t="s">
+        <v>57</v>
+      </c>
+      <c r="C35" s="3" t="s">
+        <v>59</v>
+      </c>
+      <c r="D35" s="3" t="s">
+        <v>60</v>
+      </c>
+      <c r="E35" s="3" t="s">
+        <v>61</v>
+      </c>
+      <c r="F35" s="3" t="s">
+        <v>62</v>
+      </c>
+      <c r="G35" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="H35" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="I35" s="3"/>
+    </row>
+    <row r="36" spans="1:9" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="A36" s="3" t="s">
+        <v>63</v>
+      </c>
+      <c r="B36" s="3" t="s">
+        <v>57</v>
+      </c>
+      <c r="C36" s="3" t="s">
+        <v>95</v>
+      </c>
+      <c r="D36" s="3" t="s">
+        <v>96</v>
+      </c>
+      <c r="E36" s="3" t="s">
+        <v>99</v>
+      </c>
+      <c r="F36" s="3" t="s">
+        <v>100</v>
+      </c>
+      <c r="G36" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="H36" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="I36" s="3"/>
+    </row>
+    <row r="37" spans="1:9" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="A37" s="3" t="s">
+        <v>127</v>
+      </c>
+      <c r="B37" s="3" t="s">
+        <v>57</v>
+      </c>
+      <c r="C37" s="3" t="s">
+        <v>158</v>
+      </c>
+      <c r="D37" s="3" t="s">
+        <v>159</v>
+      </c>
+      <c r="E37" s="3" t="s">
+        <v>128</v>
+      </c>
+      <c r="F37" s="3" t="s">
+        <v>129</v>
+      </c>
+      <c r="G37" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="H37" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="I37" s="3"/>
+    </row>
+    <row r="38" spans="1:9" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="A38" s="3" t="s">
+        <v>64</v>
+      </c>
+      <c r="B38" s="3" t="s">
+        <v>57</v>
+      </c>
+      <c r="C38" s="3" t="s">
+        <v>65</v>
+      </c>
+      <c r="D38" s="3" t="s">
+        <v>66</v>
+      </c>
+      <c r="E38" s="3" t="s">
+        <v>67</v>
+      </c>
+      <c r="F38" s="3" t="s">
+        <v>68</v>
+      </c>
+      <c r="G38" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="H38" s="3" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="39" spans="1:9" s="6" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="A39" s="3" t="s">
+        <v>204</v>
+      </c>
+      <c r="B39" s="3" t="s">
+        <v>69</v>
+      </c>
+      <c r="C39" s="3" t="s">
+        <v>184</v>
+      </c>
+      <c r="D39" s="3" t="s">
+        <v>185</v>
+      </c>
+      <c r="E39" s="3" t="s">
+        <v>137</v>
+      </c>
+      <c r="F39" s="3" t="s">
+        <v>138</v>
+      </c>
+      <c r="G39" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="H39" s="3" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="40" spans="1:9" s="6" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="A40" s="3" t="s">
+        <v>130</v>
+      </c>
+      <c r="B40" s="3" t="s">
+        <v>69</v>
+      </c>
+      <c r="C40" s="3" t="s">
+        <v>151</v>
+      </c>
+      <c r="D40" s="3" t="s">
+        <v>152</v>
+      </c>
+      <c r="E40" s="3" t="s">
+        <v>132</v>
+      </c>
+      <c r="F40" s="3" t="s">
+        <v>131</v>
+      </c>
+      <c r="G40" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="H40" s="3" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="41" spans="1:9" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="A41" s="3" t="s">
+        <v>70</v>
+      </c>
+      <c r="B41" s="3" t="s">
+        <v>69</v>
+      </c>
+      <c r="C41" s="3" t="s">
+        <v>133</v>
+      </c>
+      <c r="D41" s="3" t="s">
         <v>134</v>
       </c>
-      <c r="D8" s="3" t="s">
+      <c r="E41" s="5" t="s">
+        <v>71</v>
+      </c>
+      <c r="F41" s="5" t="s">
+        <v>72</v>
+      </c>
+      <c r="G41" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="H41" s="3" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="42" spans="1:9" ht="15" x14ac:dyDescent="0.25">
+      <c r="A42" s="4" t="s">
         <v>135</v>
       </c>
-      <c r="E8" s="3" t="s">
+      <c r="B42" s="3" t="s">
+        <v>69</v>
+      </c>
+      <c r="C42" s="3" t="s">
+        <v>104</v>
+      </c>
+      <c r="D42" s="3" t="s">
+        <v>103</v>
+      </c>
+      <c r="E42" s="3" t="s">
+        <v>101</v>
+      </c>
+      <c r="F42" s="3" t="s">
+        <v>102</v>
+      </c>
+      <c r="G42" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="H42" s="3" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="43" spans="1:9" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="A43" s="3" t="s">
         <v>136</v>
       </c>
-      <c r="F8" s="3" t="s">
+      <c r="B43" s="3" t="s">
+        <v>69</v>
+      </c>
+      <c r="C43" s="3" t="s">
         <v>137</v>
       </c>
-      <c r="G8" s="4" t="s">
-        <v>6</v>
-      </c>
-      <c r="H8" s="4" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="9" spans="1:9" s="6" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A9" s="3" t="s">
-        <v>113</v>
-      </c>
-      <c r="B9" s="3" t="s">
-        <v>18</v>
-      </c>
-      <c r="C9" s="3" t="s">
-        <v>19</v>
-      </c>
-      <c r="D9" s="3" t="s">
-        <v>20</v>
-      </c>
-      <c r="E9" s="3" t="s">
-        <v>121</v>
-      </c>
-      <c r="F9" s="3" t="s">
-        <v>122</v>
-      </c>
-      <c r="G9" s="4" t="s">
-        <v>6</v>
-      </c>
-      <c r="H9" s="4" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="10" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A10" s="3" t="s">
+      <c r="D43" s="3" t="s">
         <v>138</v>
       </c>
-      <c r="B10" s="3" t="s">
-        <v>18</v>
-      </c>
-      <c r="C10" s="4" t="s">
+      <c r="E43" s="3" t="s">
+        <v>153</v>
+      </c>
+      <c r="F43" s="3" t="s">
+        <v>154</v>
+      </c>
+      <c r="G43" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="H43" s="3" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="44" spans="1:9" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="A44" s="3" t="s">
         <v>139</v>
       </c>
-      <c r="D10" s="4" t="s">
+      <c r="B44" s="3" t="s">
+        <v>69</v>
+      </c>
+      <c r="C44" s="5" t="s">
+        <v>71</v>
+      </c>
+      <c r="D44" s="5" t="s">
+        <v>72</v>
+      </c>
+      <c r="E44" s="3" t="s">
+        <v>34</v>
+      </c>
+      <c r="F44" s="3" t="s">
+        <v>35</v>
+      </c>
+      <c r="G44" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="H44" s="3" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="45" spans="1:9" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="A45" s="3" t="s">
+        <v>73</v>
+      </c>
+      <c r="B45" s="3" t="s">
+        <v>69</v>
+      </c>
+      <c r="C45" s="3" t="s">
+        <v>74</v>
+      </c>
+      <c r="D45" s="3" t="s">
+        <v>75</v>
+      </c>
+      <c r="E45" s="3" t="s">
+        <v>74</v>
+      </c>
+      <c r="F45" s="3" t="s">
+        <v>75</v>
+      </c>
+      <c r="G45" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="H45" s="3" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="46" spans="1:9" s="6" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="A46" s="3" t="s">
+        <v>203</v>
+      </c>
+      <c r="B46" s="3" t="s">
+        <v>77</v>
+      </c>
+      <c r="C46" s="3" t="s">
+        <v>184</v>
+      </c>
+      <c r="D46" s="3" t="s">
+        <v>185</v>
+      </c>
+      <c r="E46" s="3" t="s">
+        <v>178</v>
+      </c>
+      <c r="F46" s="3" t="s">
+        <v>179</v>
+      </c>
+      <c r="G46" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="H46" s="3" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="47" spans="1:9" s="6" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="A47" s="3" t="s">
+        <v>76</v>
+      </c>
+      <c r="B47" s="3" t="s">
+        <v>77</v>
+      </c>
+      <c r="C47" s="3" t="s">
+        <v>78</v>
+      </c>
+      <c r="D47" s="3" t="s">
+        <v>79</v>
+      </c>
+      <c r="E47" s="3" t="s">
+        <v>78</v>
+      </c>
+      <c r="F47" s="3" t="s">
+        <v>79</v>
+      </c>
+      <c r="G47" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="H47" s="3" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="48" spans="1:9" s="6" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="A48" s="3" t="s">
+        <v>76</v>
+      </c>
+      <c r="B48" s="3" t="s">
+        <v>77</v>
+      </c>
+      <c r="C48" s="3" t="s">
+        <v>78</v>
+      </c>
+      <c r="D48" s="3" t="s">
+        <v>80</v>
+      </c>
+      <c r="E48" s="3" t="s">
+        <v>78</v>
+      </c>
+      <c r="F48" s="3" t="s">
+        <v>80</v>
+      </c>
+      <c r="G48" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="H48" s="3" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="49" spans="1:8" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="A49" s="3" t="s">
+        <v>81</v>
+      </c>
+      <c r="B49" s="3" t="s">
+        <v>77</v>
+      </c>
+      <c r="C49" s="3" t="s">
+        <v>175</v>
+      </c>
+      <c r="D49" s="3" t="s">
+        <v>176</v>
+      </c>
+      <c r="E49" s="3" t="s">
+        <v>82</v>
+      </c>
+      <c r="F49" s="3" t="s">
+        <v>83</v>
+      </c>
+      <c r="G49" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="H49" s="3" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="50" spans="1:8" s="6" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="A50" s="3" t="s">
+        <v>177</v>
+      </c>
+      <c r="B50" s="3" t="s">
+        <v>77</v>
+      </c>
+      <c r="C50" s="3" t="s">
+        <v>178</v>
+      </c>
+      <c r="D50" s="3" t="s">
+        <v>179</v>
+      </c>
+      <c r="E50" s="3" t="s">
+        <v>178</v>
+      </c>
+      <c r="F50" s="3" t="s">
+        <v>179</v>
+      </c>
+      <c r="G50" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="H50" s="3" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="51" spans="1:8" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="A51" s="3" t="s">
         <v>140</v>
       </c>
-      <c r="E10" s="4" t="s">
+      <c r="B51" s="3" t="s">
+        <v>77</v>
+      </c>
+      <c r="C51" s="3" t="s">
+        <v>87</v>
+      </c>
+      <c r="D51" s="3" t="s">
+        <v>88</v>
+      </c>
+      <c r="E51" s="3" t="s">
+        <v>89</v>
+      </c>
+      <c r="F51" s="3" t="s">
+        <v>90</v>
+      </c>
+      <c r="G51" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="H51" s="3" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="52" spans="1:8" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="A52" s="3" t="s">
+        <v>84</v>
+      </c>
+      <c r="B52" s="3" t="s">
+        <v>77</v>
+      </c>
+      <c r="C52" s="3" t="s">
+        <v>85</v>
+      </c>
+      <c r="D52" s="3" t="s">
+        <v>86</v>
+      </c>
+      <c r="E52" s="3" t="s">
+        <v>85</v>
+      </c>
+      <c r="F52" s="3" t="s">
+        <v>86</v>
+      </c>
+      <c r="G52" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="H52" s="3" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="53" spans="1:8" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="A53" s="3" t="s">
+        <v>141</v>
+      </c>
+      <c r="B53" s="3" t="s">
+        <v>77</v>
+      </c>
+      <c r="C53" s="6" t="s">
+        <v>147</v>
+      </c>
+      <c r="D53" s="6" t="s">
+        <v>148</v>
+      </c>
+      <c r="E53" s="3" t="s">
         <v>142</v>
       </c>
-      <c r="F10" s="4" t="s">
-        <v>141</v>
-      </c>
-      <c r="G10" s="4" t="s">
-        <v>6</v>
-      </c>
-      <c r="H10" s="4" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="11" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A11" s="3" t="s">
-        <v>26</v>
-      </c>
-      <c r="B11" s="3" t="s">
-        <v>27</v>
-      </c>
-      <c r="C11" s="3" t="s">
-        <v>28</v>
-      </c>
-      <c r="D11" s="3" t="s">
-        <v>29</v>
-      </c>
-      <c r="E11" s="3" t="s">
-        <v>127</v>
-      </c>
-      <c r="F11" s="3" t="s">
-        <v>128</v>
-      </c>
-      <c r="G11" s="4" t="s">
-        <v>6</v>
-      </c>
-      <c r="H11" s="4" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="12" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A12" s="3" t="s">
-        <v>30</v>
-      </c>
-      <c r="B12" s="3" t="s">
-        <v>27</v>
-      </c>
-      <c r="C12" s="3" t="s">
-        <v>31</v>
-      </c>
-      <c r="D12" s="3" t="s">
-        <v>32</v>
-      </c>
-      <c r="E12" s="3" t="s">
-        <v>33</v>
-      </c>
-      <c r="F12" s="3" t="s">
-        <v>34</v>
-      </c>
-      <c r="G12" s="3" t="s">
-        <v>35</v>
-      </c>
-      <c r="H12" s="3" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="13" spans="1:9" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="A13" s="3" t="s">
-        <v>39</v>
-      </c>
-      <c r="B13" s="3" t="s">
-        <v>27</v>
-      </c>
-      <c r="C13" s="3" t="s">
-        <v>40</v>
-      </c>
-      <c r="D13" s="3" t="s">
-        <v>41</v>
-      </c>
-      <c r="E13" s="3" t="s">
-        <v>35</v>
-      </c>
-      <c r="F13" s="3" t="s">
-        <v>36</v>
-      </c>
-      <c r="G13" s="3" t="s">
-        <v>6</v>
-      </c>
-      <c r="H13" s="3" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="14" spans="1:9" s="6" customFormat="1" ht="15" x14ac:dyDescent="0.25">
-      <c r="A14" s="4" t="s">
-        <v>42</v>
-      </c>
-      <c r="B14" s="3" t="s">
-        <v>27</v>
-      </c>
-      <c r="C14" s="4" t="s">
+      <c r="F53" s="3" t="s">
+        <v>143</v>
+      </c>
+      <c r="G53" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="H53" s="3" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="54" spans="1:8" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="A54" s="3" t="s">
         <v>144</v>
       </c>
-      <c r="D14" s="4" t="s">
+      <c r="B54" s="3" t="s">
+        <v>77</v>
+      </c>
+      <c r="C54" t="s">
         <v>145</v>
       </c>
-      <c r="E14" s="4" t="s">
-        <v>144</v>
-      </c>
-      <c r="F14" s="4" t="s">
-        <v>145</v>
-      </c>
-      <c r="G14" s="3" t="s">
-        <v>6</v>
-      </c>
-      <c r="H14" s="3" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="15" spans="1:9" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="A15" s="3" t="s">
+      <c r="D54" t="s">
         <v>146</v>
       </c>
-      <c r="B15" s="3" t="s">
-        <v>27</v>
-      </c>
-      <c r="C15" s="3" t="s">
-        <v>43</v>
-      </c>
-      <c r="D15" s="3" t="s">
-        <v>44</v>
-      </c>
-      <c r="E15" s="3" t="s">
-        <v>43</v>
-      </c>
-      <c r="F15" s="3" t="s">
-        <v>44</v>
-      </c>
-      <c r="G15" s="3" t="s">
-        <v>6</v>
-      </c>
-      <c r="H15" s="3" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="16" spans="1:9" s="6" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="A16" s="3" t="s">
-        <v>45</v>
-      </c>
-      <c r="B16" s="3" t="s">
-        <v>46</v>
-      </c>
-      <c r="C16" s="3" t="s">
-        <v>47</v>
-      </c>
-      <c r="D16" s="3" t="s">
-        <v>48</v>
-      </c>
-      <c r="E16" s="3" t="s">
-        <v>109</v>
-      </c>
-      <c r="F16" s="3" t="s">
-        <v>110</v>
-      </c>
-      <c r="G16" s="3" t="s">
-        <v>6</v>
-      </c>
-      <c r="H16" s="3" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="17" spans="1:9" ht="15" x14ac:dyDescent="0.25">
-      <c r="A17" s="4" t="s">
+      <c r="E54" s="6" t="s">
         <v>147</v>
       </c>
-      <c r="B17" s="3" t="s">
-        <v>46</v>
-      </c>
-      <c r="C17" s="4" t="s">
-        <v>37</v>
-      </c>
-      <c r="D17" s="4" t="s">
-        <v>38</v>
-      </c>
-      <c r="E17" s="3" t="s">
-        <v>52</v>
-      </c>
-      <c r="F17" s="3" t="s">
-        <v>53</v>
-      </c>
-      <c r="G17" s="4" t="s">
-        <v>6</v>
-      </c>
-      <c r="H17" s="3" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="18" spans="1:9" ht="15" x14ac:dyDescent="0.25">
-      <c r="A18" s="3" t="s">
+      <c r="F54" s="6" t="s">
         <v>148</v>
       </c>
-      <c r="B18" s="3" t="s">
-        <v>46</v>
-      </c>
-      <c r="C18" s="3" t="s">
-        <v>149</v>
-      </c>
-      <c r="D18" s="3" t="s">
-        <v>150</v>
-      </c>
-      <c r="E18" s="3" t="s">
-        <v>174</v>
-      </c>
-      <c r="F18" s="3" t="s">
-        <v>175</v>
-      </c>
-      <c r="G18" s="4" t="s">
-        <v>6</v>
-      </c>
-      <c r="H18" s="3" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="19" spans="1:9" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="A19" s="3" t="s">
-        <v>49</v>
-      </c>
-      <c r="B19" s="3" t="s">
-        <v>46</v>
-      </c>
-      <c r="C19" s="3" t="s">
-        <v>50</v>
-      </c>
-      <c r="D19" s="3" t="s">
-        <v>51</v>
-      </c>
-      <c r="E19" s="3" t="s">
-        <v>119</v>
-      </c>
-      <c r="F19" s="3" t="s">
-        <v>120</v>
-      </c>
-      <c r="G19" s="3" t="s">
-        <v>6</v>
-      </c>
-      <c r="H19" s="3" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="20" spans="1:9" ht="15" x14ac:dyDescent="0.25">
-      <c r="A20" s="4" t="s">
-        <v>54</v>
-      </c>
-      <c r="B20" s="3" t="s">
-        <v>55</v>
-      </c>
-      <c r="C20" s="3" t="s">
-        <v>56</v>
-      </c>
-      <c r="D20" s="3" t="s">
-        <v>57</v>
-      </c>
-      <c r="E20" s="3" t="s">
-        <v>58</v>
-      </c>
-      <c r="F20" s="3" t="s">
-        <v>59</v>
-      </c>
-      <c r="G20" s="3" t="s">
-        <v>6</v>
-      </c>
-      <c r="H20" s="3" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="21" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A21" s="4" t="s">
-        <v>60</v>
-      </c>
-      <c r="B21" s="3" t="s">
-        <v>55</v>
-      </c>
-      <c r="C21" s="4" t="s">
-        <v>61</v>
-      </c>
-      <c r="D21" s="4" t="s">
-        <v>62</v>
-      </c>
-      <c r="E21" s="4" t="s">
-        <v>63</v>
-      </c>
-      <c r="F21" s="4" t="s">
-        <v>64</v>
-      </c>
-      <c r="G21" s="3" t="s">
-        <v>123</v>
-      </c>
-      <c r="H21" s="3" t="s">
-        <v>124</v>
-      </c>
-    </row>
-    <row r="22" spans="1:9" ht="15" x14ac:dyDescent="0.25">
-      <c r="A22" s="4" t="s">
-        <v>151</v>
-      </c>
-      <c r="B22" s="3" t="s">
-        <v>55</v>
-      </c>
-      <c r="C22" s="3" t="s">
-        <v>123</v>
-      </c>
-      <c r="D22" s="3" t="s">
-        <v>124</v>
-      </c>
-      <c r="E22" s="3" t="s">
-        <v>125</v>
-      </c>
-      <c r="F22" s="3" t="s">
-        <v>126</v>
-      </c>
-      <c r="G22" s="3" t="s">
-        <v>6</v>
-      </c>
-      <c r="H22" s="3" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="23" spans="1:9" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="A23" s="3" t="s">
-        <v>66</v>
-      </c>
-      <c r="B23" s="3" t="s">
-        <v>65</v>
-      </c>
-      <c r="C23" s="3" t="s">
-        <v>67</v>
-      </c>
-      <c r="D23" s="3" t="s">
-        <v>68</v>
-      </c>
-      <c r="E23" s="3" t="s">
-        <v>69</v>
-      </c>
-      <c r="F23" s="3" t="s">
-        <v>70</v>
-      </c>
-      <c r="G23" s="3" t="s">
-        <v>6</v>
-      </c>
-      <c r="H23" s="3" t="s">
-        <v>6</v>
-      </c>
-      <c r="I23" s="3"/>
-    </row>
-    <row r="24" spans="1:9" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="A24" s="3" t="s">
-        <v>71</v>
-      </c>
-      <c r="B24" s="3" t="s">
-        <v>65</v>
-      </c>
-      <c r="C24" s="3" t="s">
-        <v>107</v>
-      </c>
-      <c r="D24" s="3" t="s">
-        <v>108</v>
-      </c>
-      <c r="E24" s="3" t="s">
-        <v>111</v>
-      </c>
-      <c r="F24" s="3" t="s">
-        <v>112</v>
-      </c>
-      <c r="G24" s="3" t="s">
-        <v>6</v>
-      </c>
-      <c r="H24" s="3" t="s">
-        <v>6</v>
-      </c>
-      <c r="I24" s="3"/>
-    </row>
-    <row r="25" spans="1:9" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="A25" s="3" t="s">
-        <v>152</v>
-      </c>
-      <c r="B25" s="3" t="s">
-        <v>65</v>
-      </c>
-      <c r="C25" s="3" t="s">
-        <v>37</v>
-      </c>
-      <c r="D25" s="3" t="s">
-        <v>38</v>
-      </c>
-      <c r="E25" s="3" t="s">
-        <v>153</v>
-      </c>
-      <c r="F25" s="3" t="s">
-        <v>154</v>
-      </c>
-      <c r="G25" s="3" t="s">
-        <v>6</v>
-      </c>
-      <c r="H25" s="3" t="s">
-        <v>6</v>
-      </c>
-      <c r="I25" s="3"/>
-    </row>
-    <row r="26" spans="1:9" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="A26" s="3" t="s">
-        <v>72</v>
-      </c>
-      <c r="B26" s="3" t="s">
-        <v>65</v>
-      </c>
-      <c r="C26" s="3" t="s">
-        <v>73</v>
-      </c>
-      <c r="D26" s="3" t="s">
-        <v>74</v>
-      </c>
-      <c r="E26" s="3" t="s">
-        <v>75</v>
-      </c>
-      <c r="F26" s="3" t="s">
-        <v>76</v>
-      </c>
-      <c r="G26" s="3" t="s">
-        <v>6</v>
-      </c>
-      <c r="H26" s="3" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="27" spans="1:9" s="6" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="A27" s="3" t="s">
+      <c r="G54" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="H54" s="3" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="55" spans="1:8" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="A55" s="3" t="s">
         <v>155</v>
       </c>
-      <c r="B27" s="3" t="s">
+      <c r="B55" s="3" t="s">
         <v>77</v>
       </c>
-      <c r="C27" s="3" t="s">
-        <v>176</v>
-      </c>
-      <c r="D27" s="3" t="s">
-        <v>177</v>
-      </c>
-      <c r="E27" s="3" t="s">
+      <c r="C55" t="s">
+        <v>156</v>
+      </c>
+      <c r="D55" t="s">
         <v>157</v>
       </c>
-      <c r="F27" s="3" t="s">
+      <c r="E55" s="6" t="s">
         <v>156</v>
       </c>
-      <c r="G27" s="3" t="s">
-        <v>6</v>
-      </c>
-      <c r="H27" s="3" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="28" spans="1:9" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="A28" s="3" t="s">
-        <v>78</v>
-      </c>
-      <c r="B28" s="3" t="s">
-        <v>77</v>
-      </c>
-      <c r="C28" s="3" t="s">
-        <v>158</v>
-      </c>
-      <c r="D28" s="3" t="s">
-        <v>159</v>
-      </c>
-      <c r="E28" s="5" t="s">
-        <v>79</v>
-      </c>
-      <c r="F28" s="5" t="s">
-        <v>80</v>
-      </c>
-      <c r="G28" s="3" t="s">
-        <v>6</v>
-      </c>
-      <c r="H28" s="3" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="29" spans="1:9" ht="15" x14ac:dyDescent="0.25">
-      <c r="A29" s="4" t="s">
-        <v>160</v>
-      </c>
-      <c r="B29" s="3" t="s">
-        <v>77</v>
-      </c>
-      <c r="C29" s="3" t="s">
-        <v>118</v>
-      </c>
-      <c r="D29" s="3" t="s">
-        <v>117</v>
-      </c>
-      <c r="E29" s="3" t="s">
-        <v>115</v>
-      </c>
-      <c r="F29" s="3" t="s">
-        <v>116</v>
-      </c>
-      <c r="G29" s="3" t="s">
-        <v>6</v>
-      </c>
-      <c r="H29" s="3" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="30" spans="1:9" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="A30" s="3" t="s">
-        <v>161</v>
-      </c>
-      <c r="B30" s="3" t="s">
-        <v>77</v>
-      </c>
-      <c r="C30" s="3" t="s">
-        <v>162</v>
-      </c>
-      <c r="D30" s="3" t="s">
-        <v>163</v>
-      </c>
-      <c r="E30" s="3" t="s">
-        <v>178</v>
-      </c>
-      <c r="F30" s="3" t="s">
-        <v>179</v>
-      </c>
-      <c r="G30" s="3" t="s">
-        <v>6</v>
-      </c>
-      <c r="H30" s="3" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="31" spans="1:9" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="A31" s="3" t="s">
-        <v>164</v>
-      </c>
-      <c r="B31" s="3" t="s">
-        <v>77</v>
-      </c>
-      <c r="C31" s="5" t="s">
-        <v>79</v>
-      </c>
-      <c r="D31" s="5" t="s">
-        <v>80</v>
-      </c>
-      <c r="E31" s="3" t="s">
-        <v>37</v>
-      </c>
-      <c r="F31" s="3" t="s">
-        <v>38</v>
-      </c>
-      <c r="G31" s="3" t="s">
-        <v>6</v>
-      </c>
-      <c r="H31" s="3" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="32" spans="1:9" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="A32" s="3" t="s">
-        <v>81</v>
-      </c>
-      <c r="B32" s="3" t="s">
-        <v>77</v>
-      </c>
-      <c r="C32" s="3" t="s">
-        <v>82</v>
-      </c>
-      <c r="D32" s="3" t="s">
-        <v>83</v>
-      </c>
-      <c r="E32" s="3" t="s">
-        <v>82</v>
-      </c>
-      <c r="F32" s="3" t="s">
-        <v>83</v>
-      </c>
-      <c r="G32" s="3" t="s">
-        <v>6</v>
-      </c>
-      <c r="H32" s="3" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="33" spans="1:8" s="6" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="A33" s="3" t="s">
-        <v>84</v>
-      </c>
-      <c r="B33" s="3" t="s">
-        <v>85</v>
-      </c>
-      <c r="C33" s="3" t="s">
-        <v>86</v>
-      </c>
-      <c r="D33" s="3" t="s">
-        <v>87</v>
-      </c>
-      <c r="E33" s="3" t="s">
-        <v>86</v>
-      </c>
-      <c r="F33" s="3" t="s">
-        <v>87</v>
-      </c>
-      <c r="G33" s="3" t="s">
-        <v>6</v>
-      </c>
-      <c r="H33" s="3" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="34" spans="1:8" s="6" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="A34" s="3" t="s">
-        <v>84</v>
-      </c>
-      <c r="B34" s="3" t="s">
-        <v>85</v>
-      </c>
-      <c r="C34" s="3" t="s">
-        <v>86</v>
-      </c>
-      <c r="D34" s="3" t="s">
-        <v>90</v>
-      </c>
-      <c r="E34" s="3" t="s">
-        <v>86</v>
-      </c>
-      <c r="F34" s="3" t="s">
-        <v>90</v>
-      </c>
-      <c r="G34" s="3" t="s">
-        <v>6</v>
-      </c>
-      <c r="H34" s="3" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="35" spans="1:8" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="A35" s="3" t="s">
-        <v>91</v>
-      </c>
-      <c r="B35" s="3" t="s">
-        <v>85</v>
-      </c>
-      <c r="C35" s="3" t="s">
-        <v>92</v>
-      </c>
-      <c r="D35" s="3" t="s">
-        <v>93</v>
-      </c>
-      <c r="E35" s="3" t="s">
-        <v>94</v>
-      </c>
-      <c r="F35" s="3" t="s">
-        <v>95</v>
-      </c>
-      <c r="G35" s="3" t="s">
-        <v>6</v>
-      </c>
-      <c r="H35" s="3" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="36" spans="1:8" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="A36" s="3" t="s">
-        <v>165</v>
-      </c>
-      <c r="B36" s="3" t="s">
-        <v>85</v>
-      </c>
-      <c r="C36" s="3" t="s">
-        <v>99</v>
-      </c>
-      <c r="D36" s="3" t="s">
-        <v>100</v>
-      </c>
-      <c r="E36" s="3" t="s">
-        <v>101</v>
-      </c>
-      <c r="F36" s="3" t="s">
-        <v>102</v>
-      </c>
-      <c r="G36" s="3" t="s">
-        <v>6</v>
-      </c>
-      <c r="H36" s="3" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="37" spans="1:8" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="A37" s="3" t="s">
-        <v>96</v>
-      </c>
-      <c r="B37" s="3" t="s">
-        <v>85</v>
-      </c>
-      <c r="C37" s="3" t="s">
-        <v>97</v>
-      </c>
-      <c r="D37" s="3" t="s">
-        <v>98</v>
-      </c>
-      <c r="E37" s="3" t="s">
-        <v>88</v>
-      </c>
-      <c r="F37" s="3" t="s">
-        <v>89</v>
-      </c>
-      <c r="G37" s="3" t="s">
-        <v>6</v>
-      </c>
-      <c r="H37" s="3" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="38" spans="1:8" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="A38" s="3" t="s">
-        <v>166</v>
-      </c>
-      <c r="B38" s="3" t="s">
-        <v>85</v>
-      </c>
-      <c r="C38" s="6" t="s">
-        <v>172</v>
-      </c>
-      <c r="D38" s="6" t="s">
-        <v>173</v>
-      </c>
-      <c r="E38" s="3" t="s">
-        <v>167</v>
-      </c>
-      <c r="F38" s="3" t="s">
-        <v>168</v>
-      </c>
-      <c r="G38" s="3" t="s">
-        <v>6</v>
-      </c>
-      <c r="H38" s="3" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="39" spans="1:8" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="A39" s="3" t="s">
-        <v>169</v>
-      </c>
-      <c r="B39" s="3" t="s">
-        <v>85</v>
-      </c>
-      <c r="C39" t="s">
-        <v>170</v>
-      </c>
-      <c r="D39" t="s">
-        <v>171</v>
-      </c>
-      <c r="E39" s="6" t="s">
-        <v>172</v>
-      </c>
-      <c r="F39" s="6" t="s">
-        <v>173</v>
-      </c>
-      <c r="G39" s="3" t="s">
-        <v>6</v>
-      </c>
-      <c r="H39" s="3" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="40" spans="1:8" ht="12.75" x14ac:dyDescent="0.2"/>
-    <row r="41" spans="1:8" ht="12.75" x14ac:dyDescent="0.2"/>
-    <row r="42" spans="1:8" ht="12.75" x14ac:dyDescent="0.2"/>
-    <row r="43" spans="1:8" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="A43" s="3"/>
-      <c r="B43" s="3"/>
-      <c r="C43" s="3"/>
-      <c r="D43" s="3"/>
-      <c r="E43" s="3"/>
-      <c r="F43" s="3"/>
-      <c r="G43" s="3"/>
-      <c r="H43" s="3"/>
-    </row>
-    <row r="44" spans="1:8" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="A44" s="3"/>
-      <c r="B44" s="3"/>
-      <c r="C44" s="3"/>
-      <c r="D44" s="3"/>
-      <c r="E44" s="3"/>
-      <c r="F44" s="3"/>
-      <c r="G44" s="3"/>
-      <c r="H44" s="3"/>
-    </row>
-    <row r="45" spans="1:8" ht="12.75" x14ac:dyDescent="0.2"/>
-    <row r="46" spans="1:8" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="A46" s="3"/>
-      <c r="B46" s="3"/>
-      <c r="C46" s="3"/>
-      <c r="D46" s="3"/>
-      <c r="E46" s="3"/>
-      <c r="F46" s="3"/>
-      <c r="G46" s="3"/>
-      <c r="H46" s="3"/>
-    </row>
-    <row r="47" spans="1:8" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="A47" s="3"/>
-      <c r="B47" s="3"/>
-      <c r="C47" s="3"/>
-      <c r="D47" s="3"/>
-      <c r="E47" s="3"/>
-      <c r="F47" s="3"/>
-      <c r="G47" s="3"/>
-      <c r="H47" s="3"/>
-    </row>
-    <row r="48" spans="1:8" s="6" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="A48" s="3"/>
-      <c r="B48" s="3"/>
-      <c r="C48" s="5"/>
-      <c r="D48" s="5"/>
-      <c r="E48" s="3"/>
-      <c r="F48" s="3"/>
-      <c r="G48" s="3"/>
-      <c r="H48" s="3"/>
-    </row>
-    <row r="49" spans="1:8" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="A49" s="3"/>
-      <c r="B49" s="3"/>
-      <c r="C49" s="3"/>
-      <c r="D49" s="3"/>
-      <c r="E49" s="3"/>
-      <c r="F49" s="3"/>
-      <c r="G49" s="3"/>
-      <c r="H49" s="3"/>
-    </row>
-    <row r="50" spans="1:8" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="A50" s="3"/>
-      <c r="B50" s="3"/>
-      <c r="C50" s="3"/>
-      <c r="D50" s="3"/>
-      <c r="E50" s="3"/>
-      <c r="F50" s="3"/>
-      <c r="G50" s="3"/>
-      <c r="H50" s="3"/>
-    </row>
-    <row r="51" spans="1:8" ht="12.75" x14ac:dyDescent="0.2"/>
-    <row r="52" spans="1:8" ht="12.75" x14ac:dyDescent="0.2"/>
-    <row r="53" spans="1:8" ht="12.75" x14ac:dyDescent="0.2"/>
-    <row r="54" spans="1:8" ht="12.75" x14ac:dyDescent="0.2"/>
-    <row r="55" spans="1:8" ht="12.75" x14ac:dyDescent="0.2"/>
+      <c r="F55" s="6" t="s">
+        <v>157</v>
+      </c>
+      <c r="G55" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="H55" s="3" t="s">
+        <v>6</v>
+      </c>
+    </row>
     <row r="56" spans="1:8" ht="12.75" x14ac:dyDescent="0.2"/>
     <row r="57" spans="1:8" ht="12.75" x14ac:dyDescent="0.2"/>
     <row r="58" spans="1:8" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="B58" s="7"/>
+      <c r="A58" s="3"/>
+      <c r="B58" s="3"/>
+      <c r="C58" s="3"/>
+      <c r="D58" s="3"/>
+      <c r="E58" s="3"/>
+      <c r="F58" s="3"/>
+      <c r="G58" s="3"/>
+      <c r="H58" s="3"/>
     </row>
     <row r="59" spans="1:8" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="B59" s="7"/>
-    </row>
-    <row r="60" spans="1:8" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="B60" s="7"/>
-    </row>
+      <c r="A59" s="3"/>
+      <c r="B59" s="3"/>
+      <c r="C59" s="3"/>
+      <c r="D59" s="3"/>
+      <c r="E59" s="3"/>
+      <c r="F59" s="3"/>
+      <c r="G59" s="3"/>
+      <c r="H59" s="3"/>
+    </row>
+    <row r="60" spans="1:8" ht="12.75" x14ac:dyDescent="0.2"/>
     <row r="61" spans="1:8" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="B61" s="7"/>
+      <c r="A61" s="3"/>
+      <c r="B61" s="3"/>
+      <c r="C61" s="3"/>
+      <c r="D61" s="3"/>
+      <c r="E61" s="3"/>
+      <c r="F61" s="3"/>
+      <c r="G61" s="3"/>
+      <c r="H61" s="3"/>
     </row>
     <row r="62" spans="1:8" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="B62" s="7"/>
-    </row>
-    <row r="63" spans="1:8" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="B63" s="7"/>
+      <c r="A62" s="3"/>
+      <c r="B62" s="3"/>
+      <c r="C62" s="3"/>
+      <c r="D62" s="3"/>
+      <c r="E62" s="3"/>
+      <c r="F62" s="3"/>
+      <c r="G62" s="3"/>
+      <c r="H62" s="3"/>
+    </row>
+    <row r="63" spans="1:8" s="6" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="A63" s="3"/>
+      <c r="B63" s="3"/>
+      <c r="C63" s="5"/>
+      <c r="D63" s="5"/>
+      <c r="E63" s="3"/>
+      <c r="F63" s="3"/>
+      <c r="G63" s="3"/>
+      <c r="H63" s="3"/>
     </row>
     <row r="64" spans="1:8" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="B64" s="7"/>
-    </row>
-    <row r="65" spans="2:2" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="B65" s="7"/>
-    </row>
-    <row r="66" spans="2:2" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="B66" s="7"/>
-    </row>
-    <row r="67" spans="2:2" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="B67" s="7"/>
-    </row>
-    <row r="68" spans="2:2" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="B68" s="7"/>
-    </row>
-    <row r="69" spans="2:2" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="B69" s="7"/>
-    </row>
-    <row r="70" spans="2:2" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="B70" s="7"/>
-    </row>
-    <row r="71" spans="2:2" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="B71" s="7"/>
-    </row>
-    <row r="72" spans="2:2" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="B72" s="7"/>
-    </row>
-    <row r="73" spans="2:2" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="A64" s="3"/>
+      <c r="B64" s="3"/>
+      <c r="C64" s="3"/>
+      <c r="D64" s="3"/>
+      <c r="E64" s="3"/>
+      <c r="F64" s="3"/>
+      <c r="G64" s="3"/>
+      <c r="H64" s="3"/>
+    </row>
+    <row r="65" spans="1:8" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="A65" s="3"/>
+      <c r="B65" s="3"/>
+      <c r="C65" s="3"/>
+      <c r="D65" s="3"/>
+      <c r="E65" s="3"/>
+      <c r="F65" s="3"/>
+      <c r="G65" s="3"/>
+      <c r="H65" s="3"/>
+    </row>
+    <row r="66" spans="1:8" ht="12.75" x14ac:dyDescent="0.2"/>
+    <row r="67" spans="1:8" ht="12.75" x14ac:dyDescent="0.2"/>
+    <row r="68" spans="1:8" ht="12.75" x14ac:dyDescent="0.2"/>
+    <row r="69" spans="1:8" ht="12.75" x14ac:dyDescent="0.2"/>
+    <row r="70" spans="1:8" ht="12.75" x14ac:dyDescent="0.2"/>
+    <row r="71" spans="1:8" ht="12.75" x14ac:dyDescent="0.2"/>
+    <row r="72" spans="1:8" ht="12.75" x14ac:dyDescent="0.2"/>
+    <row r="73" spans="1:8" ht="12.75" x14ac:dyDescent="0.2">
       <c r="B73" s="7"/>
     </row>
-    <row r="74" spans="2:2" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="74" spans="1:8" ht="12.75" x14ac:dyDescent="0.2">
       <c r="B74" s="7"/>
     </row>
-    <row r="75" spans="2:2" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="75" spans="1:8" ht="12.75" x14ac:dyDescent="0.2">
       <c r="B75" s="7"/>
     </row>
-    <row r="76" spans="2:2" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="76" spans="1:8" ht="12.75" x14ac:dyDescent="0.2">
       <c r="B76" s="7"/>
     </row>
-    <row r="77" spans="2:2" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="77" spans="1:8" ht="12.75" x14ac:dyDescent="0.2">
       <c r="B77" s="7"/>
     </row>
-    <row r="78" spans="2:2" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="78" spans="1:8" ht="12.75" x14ac:dyDescent="0.2">
       <c r="B78" s="7"/>
     </row>
-    <row r="79" spans="2:2" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="79" spans="1:8" ht="12.75" x14ac:dyDescent="0.2">
       <c r="B79" s="7"/>
     </row>
-    <row r="80" spans="2:2" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="80" spans="1:8" ht="12.75" x14ac:dyDescent="0.2">
       <c r="B80" s="7"/>
     </row>
     <row r="81" spans="2:2" ht="12.75" x14ac:dyDescent="0.2">
@@ -4806,8 +5300,54 @@
     <row r="1000" spans="2:2" ht="12.75" x14ac:dyDescent="0.2">
       <c r="B1000" s="7"/>
     </row>
+    <row r="1001" spans="2:2" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="B1001" s="7"/>
+    </row>
+    <row r="1002" spans="2:2" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="B1002" s="7"/>
+    </row>
+    <row r="1003" spans="2:2" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="B1003" s="7"/>
+    </row>
+    <row r="1004" spans="2:2" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="B1004" s="7"/>
+    </row>
+    <row r="1005" spans="2:2" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="B1005" s="7"/>
+    </row>
+    <row r="1006" spans="2:2" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="B1006" s="7"/>
+    </row>
+    <row r="1007" spans="2:2" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="B1007" s="7"/>
+    </row>
+    <row r="1008" spans="2:2" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="B1008" s="7"/>
+    </row>
+    <row r="1009" spans="2:2" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="B1009" s="7"/>
+    </row>
+    <row r="1010" spans="2:2" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="B1010" s="7"/>
+    </row>
+    <row r="1011" spans="2:2" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="B1011" s="7"/>
+    </row>
+    <row r="1012" spans="2:2" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="B1012" s="7"/>
+    </row>
+    <row r="1013" spans="2:2" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="B1013" s="7"/>
+    </row>
+    <row r="1014" spans="2:2" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="B1014" s="7"/>
+    </row>
+    <row r="1015" spans="2:2" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="B1015" s="7"/>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">
       <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="1">
@@ -4815,7 +5355,7 @@
           <x14:formula1>
             <xm:f>Class!$A$2:$A$9</xm:f>
           </x14:formula1>
-          <xm:sqref>B43:B44 B58:B1000 B46:B50 B2:B39</xm:sqref>
+          <xm:sqref>B58:B59 B73:B1015 B61:B65 B4:B55</xm:sqref>
         </x14:dataValidation>
       </x14:dataValidations>
     </ext>
@@ -4836,7 +5376,7 @@
   <sheetData>
     <row r="1" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A1" s="8" t="s">
-        <v>103</v>
+        <v>91</v>
       </c>
     </row>
     <row r="2" spans="1:1" x14ac:dyDescent="0.2">
@@ -4851,32 +5391,32 @@
     </row>
     <row r="4" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A4" s="3" t="s">
-        <v>27</v>
+        <v>24</v>
       </c>
     </row>
     <row r="5" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A5" s="3" t="s">
-        <v>46</v>
+        <v>43</v>
       </c>
     </row>
     <row r="6" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A6" s="3" t="s">
-        <v>55</v>
+        <v>49</v>
       </c>
     </row>
     <row r="7" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A7" s="3" t="s">
-        <v>65</v>
+        <v>57</v>
       </c>
     </row>
     <row r="8" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A8" s="3" t="s">
-        <v>77</v>
+        <v>69</v>
       </c>
     </row>
     <row r="9" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A9" s="3" t="s">
-        <v>85</v>
+        <v>77</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Modular version of new JCG scraper
</commit_message>
<xml_diff>
--- a/Excel_and_CSV/OmenMeta.xlsx
+++ b/Excel_and_CSV/OmenMeta.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24827"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24931"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Python_WS\Github_SV\Excel_and_CSV\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{14CA4C6F-A795-4821-8141-3276AC992648}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{64A5A3FE-757F-4EC3-BEA2-E365F12DF6ED}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20640" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="449" uniqueCount="218">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="441" uniqueCount="213">
   <si>
     <t>Archetype Name</t>
   </si>
@@ -161,12 +161,6 @@
     <t>7BSYy</t>
   </si>
   <si>
-    <t>Naterra's Future</t>
-  </si>
-  <si>
-    <t>7DjKQ</t>
-  </si>
-  <si>
     <t>Machina Shadow</t>
   </si>
   <si>
@@ -338,12 +332,6 @@
     <t>Frigg</t>
   </si>
   <si>
-    <t>Djeana, the Stouthearted</t>
-  </si>
-  <si>
-    <t>7FEFY</t>
-  </si>
-  <si>
     <t>Suzy, Hexcaster</t>
   </si>
   <si>
@@ -365,9 +353,6 @@
     <t>Piercye, Queen of Frost</t>
   </si>
   <si>
-    <t>7Hsiy</t>
-  </si>
-  <si>
     <t>7LlkS</t>
   </si>
   <si>
@@ -623,9 +608,6 @@
     <t>7NCW6</t>
   </si>
   <si>
-    <t>Natura Burn Dragon</t>
-  </si>
-  <si>
     <t>Brutal Dragonewt</t>
   </si>
   <si>
@@ -675,6 +657,9 @@
   </si>
   <si>
     <t>Evo Shadow</t>
+  </si>
+  <si>
+    <t>7Llkc</t>
   </si>
 </sst>
 </file>
@@ -982,10 +967,10 @@
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
-  <dimension ref="A1:I1015"/>
+  <dimension ref="A1:I1014"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A22" workbookViewId="0">
-      <selection activeCell="E38" sqref="E38"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E35" sqref="E35"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -1011,40 +996,40 @@
         <v>2</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
       <c r="E1" s="1" t="s">
         <v>3</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
       <c r="G1" s="1" t="s">
         <v>4</v>
       </c>
       <c r="H1" s="1" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
       <c r="I1" s="2"/>
     </row>
     <row r="2" spans="1:9" s="6" customFormat="1" ht="15" x14ac:dyDescent="0.25">
       <c r="A2" s="3" t="s">
-        <v>213</v>
+        <v>207</v>
       </c>
       <c r="B2" s="3" t="s">
         <v>5</v>
       </c>
       <c r="C2" s="3" t="s">
-        <v>184</v>
+        <v>179</v>
       </c>
       <c r="D2" s="3" t="s">
-        <v>185</v>
+        <v>180</v>
       </c>
       <c r="E2" s="1" t="s">
-        <v>209</v>
+        <v>203</v>
       </c>
       <c r="F2" s="1" t="s">
-        <v>210</v>
+        <v>204</v>
       </c>
       <c r="G2" s="4" t="s">
         <v>6</v>
@@ -1056,22 +1041,22 @@
     </row>
     <row r="3" spans="1:9" s="6" customFormat="1" ht="15" x14ac:dyDescent="0.25">
       <c r="A3" s="3" t="s">
-        <v>166</v>
+        <v>161</v>
       </c>
       <c r="B3" s="3" t="s">
         <v>5</v>
       </c>
       <c r="C3" s="4" t="s">
-        <v>113</v>
+        <v>109</v>
       </c>
       <c r="D3" s="4" t="s">
-        <v>115</v>
+        <v>110</v>
       </c>
       <c r="E3" s="4" t="s">
-        <v>167</v>
+        <v>162</v>
       </c>
       <c r="F3" s="4" t="s">
-        <v>114</v>
+        <v>212</v>
       </c>
       <c r="G3" s="4" t="s">
         <v>12</v>
@@ -1083,22 +1068,22 @@
     </row>
     <row r="4" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="3" t="s">
-        <v>166</v>
+        <v>161</v>
       </c>
       <c r="B4" s="3" t="s">
         <v>5</v>
       </c>
       <c r="C4" s="4" t="s">
-        <v>113</v>
+        <v>109</v>
       </c>
       <c r="D4" s="4" t="s">
-        <v>115</v>
+        <v>110</v>
       </c>
       <c r="E4" s="4" t="s">
-        <v>167</v>
+        <v>162</v>
       </c>
       <c r="F4" s="4" t="s">
-        <v>114</v>
+        <v>212</v>
       </c>
       <c r="G4" s="4" t="s">
         <v>12</v>
@@ -1109,7 +1094,7 @@
     </row>
     <row r="5" spans="1:9" s="6" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="3" t="s">
-        <v>160</v>
+        <v>155</v>
       </c>
       <c r="B5" s="3" t="s">
         <v>5</v>
@@ -1135,7 +1120,7 @@
     </row>
     <row r="6" spans="1:9" s="6" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="3" t="s">
-        <v>160</v>
+        <v>155</v>
       </c>
       <c r="B6" s="3" t="s">
         <v>5</v>
@@ -1213,7 +1198,7 @@
     </row>
     <row r="9" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9" s="3" t="s">
-        <v>116</v>
+        <v>111</v>
       </c>
       <c r="B9" s="3" t="s">
         <v>5</v>
@@ -1265,16 +1250,16 @@
     </row>
     <row r="11" spans="1:9" s="6" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A11" s="3" t="s">
-        <v>186</v>
+        <v>181</v>
       </c>
       <c r="B11" s="3" t="s">
         <v>18</v>
       </c>
       <c r="C11" s="3" t="s">
-        <v>184</v>
+        <v>179</v>
       </c>
       <c r="D11" s="3" t="s">
-        <v>185</v>
+        <v>180</v>
       </c>
       <c r="E11" s="4" t="s">
         <v>19</v>
@@ -1291,16 +1276,16 @@
     </row>
     <row r="12" spans="1:9" s="6" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A12" s="3" t="s">
-        <v>180</v>
+        <v>175</v>
       </c>
       <c r="B12" s="3" t="s">
         <v>18</v>
       </c>
       <c r="C12" s="9" t="s">
-        <v>181</v>
+        <v>176</v>
       </c>
       <c r="D12" s="4" t="s">
-        <v>182</v>
+        <v>177</v>
       </c>
       <c r="E12" s="4" t="s">
         <v>21</v>
@@ -1309,82 +1294,82 @@
         <v>22</v>
       </c>
       <c r="G12" s="3" t="s">
-        <v>117</v>
+        <v>112</v>
       </c>
       <c r="H12" s="3" t="s">
-        <v>118</v>
+        <v>113</v>
       </c>
     </row>
     <row r="13" spans="1:9" s="6" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A13" s="3" t="s">
-        <v>161</v>
+        <v>156</v>
       </c>
       <c r="B13" s="3" t="s">
         <v>18</v>
       </c>
       <c r="C13" s="9" t="s">
-        <v>188</v>
+        <v>183</v>
       </c>
       <c r="D13" s="4" t="s">
-        <v>189</v>
+        <v>184</v>
       </c>
       <c r="E13" s="4" t="s">
-        <v>162</v>
+        <v>157</v>
       </c>
       <c r="F13" s="4" t="s">
-        <v>163</v>
+        <v>158</v>
       </c>
       <c r="G13" s="3" t="s">
-        <v>190</v>
+        <v>185</v>
       </c>
       <c r="H13" s="3" t="s">
-        <v>191</v>
+        <v>186</v>
       </c>
     </row>
     <row r="14" spans="1:9" s="6" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A14" s="3" t="s">
-        <v>214</v>
+        <v>208</v>
       </c>
       <c r="B14" s="3" t="s">
         <v>18</v>
       </c>
       <c r="C14" s="9" t="s">
-        <v>215</v>
+        <v>209</v>
       </c>
       <c r="D14" s="4" t="s">
-        <v>216</v>
+        <v>210</v>
       </c>
       <c r="E14" s="3" t="s">
-        <v>190</v>
+        <v>185</v>
       </c>
       <c r="F14" s="3" t="s">
-        <v>191</v>
+        <v>186</v>
       </c>
       <c r="G14" s="3" t="s">
-        <v>117</v>
+        <v>112</v>
       </c>
       <c r="H14" s="3" t="s">
-        <v>118</v>
+        <v>113</v>
       </c>
     </row>
     <row r="15" spans="1:9" s="6" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A15" s="3" t="s">
-        <v>187</v>
+        <v>182</v>
       </c>
       <c r="B15" s="3" t="s">
         <v>18</v>
       </c>
       <c r="C15" s="3" t="s">
-        <v>190</v>
+        <v>185</v>
       </c>
       <c r="D15" s="3" t="s">
-        <v>191</v>
+        <v>186</v>
       </c>
       <c r="E15" s="3" t="s">
-        <v>190</v>
+        <v>185</v>
       </c>
       <c r="F15" s="3" t="s">
-        <v>191</v>
+        <v>186</v>
       </c>
       <c r="G15" s="3" t="s">
         <v>6</v>
@@ -1395,22 +1380,22 @@
     </row>
     <row r="16" spans="1:9" s="6" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A16" s="3" t="s">
-        <v>187</v>
+        <v>182</v>
       </c>
       <c r="B16" s="3" t="s">
         <v>18</v>
       </c>
       <c r="C16" s="9" t="s">
-        <v>119</v>
+        <v>114</v>
       </c>
       <c r="D16" s="4" t="s">
-        <v>120</v>
+        <v>115</v>
       </c>
       <c r="E16" s="9" t="s">
-        <v>119</v>
+        <v>114</v>
       </c>
       <c r="F16" s="4" t="s">
-        <v>120</v>
+        <v>115</v>
       </c>
       <c r="G16" s="3" t="s">
         <v>6</v>
@@ -1421,16 +1406,16 @@
     </row>
     <row r="17" spans="1:8" s="6" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A17" s="3" t="s">
-        <v>208</v>
+        <v>202</v>
       </c>
       <c r="B17" s="3" t="s">
         <v>24</v>
       </c>
       <c r="C17" s="3" t="s">
-        <v>184</v>
+        <v>179</v>
       </c>
       <c r="D17" s="3" t="s">
-        <v>185</v>
+        <v>180</v>
       </c>
       <c r="E17" s="3" t="s">
         <v>37</v>
@@ -1459,10 +1444,10 @@
         <v>26</v>
       </c>
       <c r="E18" s="3" t="s">
-        <v>111</v>
+        <v>107</v>
       </c>
       <c r="F18" s="3" t="s">
-        <v>112</v>
+        <v>108</v>
       </c>
       <c r="G18" s="4" t="s">
         <v>6</v>
@@ -1511,10 +1496,10 @@
         <v>38</v>
       </c>
       <c r="E20" s="3" t="s">
-        <v>168</v>
+        <v>163</v>
       </c>
       <c r="F20" s="3" t="s">
-        <v>169</v>
+        <v>164</v>
       </c>
       <c r="G20" s="3" t="s">
         <v>6</v>
@@ -1531,16 +1516,16 @@
         <v>24</v>
       </c>
       <c r="C21" s="4" t="s">
-        <v>121</v>
+        <v>116</v>
       </c>
       <c r="D21" s="4" t="s">
-        <v>122</v>
+        <v>117</v>
       </c>
       <c r="E21" s="4" t="s">
-        <v>121</v>
+        <v>116</v>
       </c>
       <c r="F21" s="4" t="s">
-        <v>122</v>
+        <v>117</v>
       </c>
       <c r="G21" s="3" t="s">
         <v>6</v>
@@ -1551,7 +1536,7 @@
     </row>
     <row r="22" spans="1:8" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A22" s="3" t="s">
-        <v>123</v>
+        <v>118</v>
       </c>
       <c r="B22" s="3" t="s">
         <v>24</v>
@@ -1577,22 +1562,22 @@
     </row>
     <row r="23" spans="1:8" s="6" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A23" s="3" t="s">
-        <v>183</v>
+        <v>178</v>
       </c>
       <c r="B23" s="3" t="s">
         <v>43</v>
       </c>
       <c r="C23" s="3" t="s">
-        <v>184</v>
+        <v>179</v>
       </c>
       <c r="D23" s="3" t="s">
-        <v>185</v>
+        <v>180</v>
       </c>
       <c r="E23" s="3" t="s">
-        <v>201</v>
+        <v>195</v>
       </c>
       <c r="F23" s="3" t="s">
-        <v>202</v>
+        <v>196</v>
       </c>
       <c r="G23" s="3" t="s">
         <v>6</v>
@@ -1615,10 +1600,10 @@
         <v>45</v>
       </c>
       <c r="E24" s="3" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
       <c r="F24" s="3" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
       <c r="G24" s="3" t="s">
         <v>6</v>
@@ -1629,178 +1614,178 @@
     </row>
     <row r="25" spans="1:8" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A25" s="3" t="s">
-        <v>124</v>
+        <v>119</v>
       </c>
       <c r="B25" s="3" t="s">
         <v>43</v>
       </c>
       <c r="C25" s="3" t="s">
-        <v>125</v>
+        <v>120</v>
       </c>
       <c r="D25" s="3" t="s">
-        <v>126</v>
+        <v>121</v>
       </c>
       <c r="E25" s="3" t="s">
-        <v>149</v>
+        <v>144</v>
       </c>
       <c r="F25" s="3" t="s">
-        <v>150</v>
+        <v>145</v>
       </c>
       <c r="G25" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="H25" s="3" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="26" spans="1:8" s="6" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="A26" s="3" t="s">
+        <v>199</v>
+      </c>
+      <c r="B26" s="3" t="s">
+        <v>47</v>
+      </c>
+      <c r="C26" s="3" t="s">
+        <v>179</v>
+      </c>
+      <c r="D26" s="3" t="s">
+        <v>180</v>
+      </c>
+      <c r="E26" s="3" t="s">
+        <v>201</v>
+      </c>
+      <c r="F26" s="3" t="s">
+        <v>200</v>
+      </c>
+      <c r="G26" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="H26" s="3" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="27" spans="1:8" ht="15" x14ac:dyDescent="0.25">
+      <c r="A27" s="4" t="s">
         <v>46</v>
       </c>
-      <c r="H25" s="3" t="s">
+      <c r="B27" s="3" t="s">
         <v>47</v>
       </c>
-    </row>
-    <row r="26" spans="1:8" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="A26" s="3" t="s">
-        <v>200</v>
-      </c>
-      <c r="B26" s="3" t="s">
-        <v>43</v>
-      </c>
-      <c r="C26" s="3" t="s">
-        <v>46</v>
-      </c>
-      <c r="D26" s="3" t="s">
+      <c r="C27" s="3" t="s">
+        <v>48</v>
+      </c>
+      <c r="D27" s="3" t="s">
+        <v>49</v>
+      </c>
+      <c r="E27" s="3" t="s">
+        <v>50</v>
+      </c>
+      <c r="F27" s="3" t="s">
+        <v>51</v>
+      </c>
+      <c r="G27" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="H27" s="3" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="28" spans="1:8" s="6" customFormat="1" ht="15" x14ac:dyDescent="0.25">
+      <c r="A28" s="4" t="s">
+        <v>165</v>
+      </c>
+      <c r="B28" s="3" t="s">
         <v>47</v>
       </c>
-      <c r="E26" s="3" t="s">
+      <c r="C28" s="3" t="s">
+        <v>166</v>
+      </c>
+      <c r="D28" s="3" t="s">
+        <v>167</v>
+      </c>
+      <c r="E28" s="3" t="s">
+        <v>169</v>
+      </c>
+      <c r="F28" s="3" t="s">
+        <v>168</v>
+      </c>
+      <c r="G28" s="4" t="s">
+        <v>159</v>
+      </c>
+      <c r="H28" s="4" t="s">
+        <v>160</v>
+      </c>
+    </row>
+    <row r="29" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A29" s="4" t="s">
+        <v>52</v>
+      </c>
+      <c r="B29" s="3" t="s">
+        <v>47</v>
+      </c>
+      <c r="C29" s="4" t="s">
+        <v>53</v>
+      </c>
+      <c r="D29" s="4" t="s">
+        <v>54</v>
+      </c>
+      <c r="E29" s="4" t="s">
+        <v>159</v>
+      </c>
+      <c r="F29" s="4" t="s">
+        <v>160</v>
+      </c>
+      <c r="G29" s="3" t="s">
         <v>105</v>
       </c>
-      <c r="F26" s="3" t="s">
+      <c r="H29" s="3" t="s">
         <v>106</v>
       </c>
-      <c r="G26" s="3" t="s">
-        <v>6</v>
-      </c>
-      <c r="H26" s="3" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="27" spans="1:8" s="6" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="A27" s="3" t="s">
-        <v>205</v>
-      </c>
-      <c r="B27" s="3" t="s">
-        <v>49</v>
-      </c>
-      <c r="C27" s="3" t="s">
-        <v>184</v>
-      </c>
-      <c r="D27" s="3" t="s">
-        <v>185</v>
-      </c>
-      <c r="E27" s="3" t="s">
-        <v>207</v>
-      </c>
-      <c r="F27" s="3" t="s">
-        <v>206</v>
-      </c>
-      <c r="G27" s="3" t="s">
-        <v>6</v>
-      </c>
-      <c r="H27" s="3" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="28" spans="1:8" ht="15" x14ac:dyDescent="0.25">
-      <c r="A28" s="4" t="s">
-        <v>48</v>
-      </c>
-      <c r="B28" s="3" t="s">
-        <v>49</v>
-      </c>
-      <c r="C28" s="3" t="s">
-        <v>50</v>
-      </c>
-      <c r="D28" s="3" t="s">
-        <v>51</v>
-      </c>
-      <c r="E28" s="3" t="s">
-        <v>52</v>
-      </c>
-      <c r="F28" s="3" t="s">
-        <v>53</v>
-      </c>
-      <c r="G28" s="3" t="s">
-        <v>6</v>
-      </c>
-      <c r="H28" s="3" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="29" spans="1:8" s="6" customFormat="1" ht="15" x14ac:dyDescent="0.25">
-      <c r="A29" s="4" t="s">
-        <v>170</v>
-      </c>
-      <c r="B29" s="3" t="s">
-        <v>49</v>
-      </c>
-      <c r="C29" s="3" t="s">
-        <v>171</v>
-      </c>
-      <c r="D29" s="3" t="s">
-        <v>172</v>
-      </c>
-      <c r="E29" s="3" t="s">
-        <v>174</v>
-      </c>
-      <c r="F29" s="3" t="s">
-        <v>173</v>
-      </c>
-      <c r="G29" s="4" t="s">
-        <v>164</v>
-      </c>
-      <c r="H29" s="4" t="s">
-        <v>165</v>
-      </c>
-    </row>
-    <row r="30" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    </row>
+    <row r="30" spans="1:8" ht="15" x14ac:dyDescent="0.25">
       <c r="A30" s="4" t="s">
-        <v>54</v>
+        <v>211</v>
       </c>
       <c r="B30" s="3" t="s">
-        <v>49</v>
-      </c>
-      <c r="C30" s="4" t="s">
-        <v>55</v>
-      </c>
-      <c r="D30" s="4" t="s">
-        <v>56</v>
-      </c>
-      <c r="E30" s="4" t="s">
-        <v>164</v>
-      </c>
-      <c r="F30" s="4" t="s">
-        <v>165</v>
+        <v>47</v>
+      </c>
+      <c r="C30" s="3" t="s">
+        <v>103</v>
+      </c>
+      <c r="D30" s="3" t="s">
+        <v>104</v>
+      </c>
+      <c r="E30" s="3" t="s">
+        <v>105</v>
+      </c>
+      <c r="F30" s="3" t="s">
+        <v>106</v>
       </c>
       <c r="G30" s="3" t="s">
-        <v>109</v>
+        <v>6</v>
       </c>
       <c r="H30" s="3" t="s">
-        <v>110</v>
-      </c>
-    </row>
-    <row r="31" spans="1:8" ht="15" x14ac:dyDescent="0.25">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="31" spans="1:8" s="6" customFormat="1" ht="15" x14ac:dyDescent="0.25">
       <c r="A31" s="4" t="s">
-        <v>217</v>
+        <v>190</v>
       </c>
       <c r="B31" s="3" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="C31" s="3" t="s">
-        <v>107</v>
+        <v>191</v>
       </c>
       <c r="D31" s="3" t="s">
-        <v>108</v>
+        <v>192</v>
       </c>
       <c r="E31" s="3" t="s">
-        <v>109</v>
+        <v>193</v>
       </c>
       <c r="F31" s="3" t="s">
-        <v>110</v>
+        <v>194</v>
       </c>
       <c r="G31" s="3" t="s">
         <v>6</v>
@@ -1811,22 +1796,22 @@
     </row>
     <row r="32" spans="1:8" s="6" customFormat="1" ht="15" x14ac:dyDescent="0.25">
       <c r="A32" s="4" t="s">
-        <v>195</v>
+        <v>52</v>
       </c>
       <c r="B32" s="3" t="s">
-        <v>49</v>
-      </c>
-      <c r="C32" s="3" t="s">
-        <v>196</v>
-      </c>
-      <c r="D32" s="3" t="s">
-        <v>197</v>
+        <v>47</v>
+      </c>
+      <c r="C32" s="4" t="s">
+        <v>53</v>
+      </c>
+      <c r="D32" s="4" t="s">
+        <v>54</v>
       </c>
       <c r="E32" s="3" t="s">
-        <v>198</v>
+        <v>205</v>
       </c>
       <c r="F32" s="3" t="s">
-        <v>199</v>
+        <v>206</v>
       </c>
       <c r="G32" s="3" t="s">
         <v>6</v>
@@ -1837,48 +1822,48 @@
     </row>
     <row r="33" spans="1:9" s="6" customFormat="1" ht="15" x14ac:dyDescent="0.25">
       <c r="A33" s="4" t="s">
-        <v>54</v>
+        <v>187</v>
       </c>
       <c r="B33" s="3" t="s">
-        <v>49</v>
-      </c>
-      <c r="C33" s="4" t="s">
         <v>55</v>
       </c>
-      <c r="D33" s="4" t="s">
+      <c r="C33" s="3" t="s">
+        <v>179</v>
+      </c>
+      <c r="D33" s="3" t="s">
+        <v>180</v>
+      </c>
+      <c r="E33" s="3" t="s">
+        <v>189</v>
+      </c>
+      <c r="F33" s="3" t="s">
+        <v>188</v>
+      </c>
+      <c r="G33" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="H33" s="3" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="34" spans="1:9" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="A34" s="3" t="s">
         <v>56</v>
       </c>
-      <c r="E33" s="3" t="s">
-        <v>211</v>
-      </c>
-      <c r="F33" s="3" t="s">
-        <v>212</v>
-      </c>
-      <c r="G33" s="3" t="s">
-        <v>6</v>
-      </c>
-      <c r="H33" s="3" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="34" spans="1:9" s="6" customFormat="1" ht="15" x14ac:dyDescent="0.25">
-      <c r="A34" s="4" t="s">
-        <v>192</v>
-      </c>
       <c r="B34" s="3" t="s">
+        <v>55</v>
+      </c>
+      <c r="C34" s="3" t="s">
         <v>57</v>
       </c>
-      <c r="C34" s="3" t="s">
-        <v>184</v>
-      </c>
       <c r="D34" s="3" t="s">
-        <v>185</v>
+        <v>58</v>
       </c>
       <c r="E34" s="3" t="s">
-        <v>194</v>
+        <v>59</v>
       </c>
       <c r="F34" s="3" t="s">
-        <v>193</v>
+        <v>60</v>
       </c>
       <c r="G34" s="3" t="s">
         <v>6</v>
@@ -1886,25 +1871,26 @@
       <c r="H34" s="3" t="s">
         <v>6</v>
       </c>
+      <c r="I34" s="3"/>
     </row>
     <row r="35" spans="1:9" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A35" s="3" t="s">
-        <v>58</v>
+        <v>61</v>
       </c>
       <c r="B35" s="3" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="C35" s="3" t="s">
-        <v>59</v>
+        <v>93</v>
       </c>
       <c r="D35" s="3" t="s">
-        <v>60</v>
+        <v>94</v>
       </c>
       <c r="E35" s="3" t="s">
-        <v>61</v>
+        <v>97</v>
       </c>
       <c r="F35" s="3" t="s">
-        <v>62</v>
+        <v>98</v>
       </c>
       <c r="G35" s="3" t="s">
         <v>6</v>
@@ -1916,22 +1902,22 @@
     </row>
     <row r="36" spans="1:9" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A36" s="3" t="s">
-        <v>63</v>
+        <v>122</v>
       </c>
       <c r="B36" s="3" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="C36" s="3" t="s">
-        <v>95</v>
+        <v>153</v>
       </c>
       <c r="D36" s="3" t="s">
-        <v>96</v>
+        <v>154</v>
       </c>
       <c r="E36" s="3" t="s">
-        <v>99</v>
+        <v>123</v>
       </c>
       <c r="F36" s="3" t="s">
-        <v>100</v>
+        <v>124</v>
       </c>
       <c r="G36" s="3" t="s">
         <v>6</v>
@@ -1943,22 +1929,22 @@
     </row>
     <row r="37" spans="1:9" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A37" s="3" t="s">
-        <v>127</v>
+        <v>62</v>
       </c>
       <c r="B37" s="3" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="C37" s="3" t="s">
-        <v>158</v>
+        <v>63</v>
       </c>
       <c r="D37" s="3" t="s">
-        <v>159</v>
+        <v>64</v>
       </c>
       <c r="E37" s="3" t="s">
-        <v>128</v>
+        <v>65</v>
       </c>
       <c r="F37" s="3" t="s">
-        <v>129</v>
+        <v>66</v>
       </c>
       <c r="G37" s="3" t="s">
         <v>6</v>
@@ -1966,26 +1952,25 @@
       <c r="H37" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="I37" s="3"/>
-    </row>
-    <row r="38" spans="1:9" ht="12.75" x14ac:dyDescent="0.2">
+    </row>
+    <row r="38" spans="1:9" s="6" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A38" s="3" t="s">
-        <v>64</v>
+        <v>198</v>
       </c>
       <c r="B38" s="3" t="s">
-        <v>57</v>
+        <v>67</v>
       </c>
       <c r="C38" s="3" t="s">
-        <v>65</v>
+        <v>179</v>
       </c>
       <c r="D38" s="3" t="s">
-        <v>66</v>
+        <v>180</v>
       </c>
       <c r="E38" s="3" t="s">
-        <v>67</v>
+        <v>132</v>
       </c>
       <c r="F38" s="3" t="s">
-        <v>68</v>
+        <v>133</v>
       </c>
       <c r="G38" s="3" t="s">
         <v>6</v>
@@ -1996,100 +1981,100 @@
     </row>
     <row r="39" spans="1:9" s="6" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A39" s="3" t="s">
-        <v>204</v>
+        <v>125</v>
       </c>
       <c r="B39" s="3" t="s">
+        <v>67</v>
+      </c>
+      <c r="C39" s="3" t="s">
+        <v>146</v>
+      </c>
+      <c r="D39" s="3" t="s">
+        <v>147</v>
+      </c>
+      <c r="E39" s="3" t="s">
+        <v>127</v>
+      </c>
+      <c r="F39" s="3" t="s">
+        <v>126</v>
+      </c>
+      <c r="G39" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="H39" s="3" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="40" spans="1:9" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="A40" s="3" t="s">
+        <v>68</v>
+      </c>
+      <c r="B40" s="3" t="s">
+        <v>67</v>
+      </c>
+      <c r="C40" s="3" t="s">
+        <v>128</v>
+      </c>
+      <c r="D40" s="3" t="s">
+        <v>129</v>
+      </c>
+      <c r="E40" s="5" t="s">
         <v>69</v>
       </c>
-      <c r="C39" s="3" t="s">
-        <v>184</v>
-      </c>
-      <c r="D39" s="3" t="s">
-        <v>185</v>
-      </c>
-      <c r="E39" s="3" t="s">
-        <v>137</v>
-      </c>
-      <c r="F39" s="3" t="s">
-        <v>138</v>
-      </c>
-      <c r="G39" s="3" t="s">
-        <v>6</v>
-      </c>
-      <c r="H39" s="3" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="40" spans="1:9" s="6" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="A40" s="3" t="s">
+      <c r="F40" s="5" t="s">
+        <v>70</v>
+      </c>
+      <c r="G40" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="H40" s="3" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="41" spans="1:9" ht="15" x14ac:dyDescent="0.25">
+      <c r="A41" s="4" t="s">
         <v>130</v>
       </c>
-      <c r="B40" s="3" t="s">
-        <v>69</v>
-      </c>
-      <c r="C40" s="3" t="s">
-        <v>151</v>
-      </c>
-      <c r="D40" s="3" t="s">
-        <v>152</v>
-      </c>
-      <c r="E40" s="3" t="s">
+      <c r="B41" s="3" t="s">
+        <v>67</v>
+      </c>
+      <c r="C41" s="3" t="s">
+        <v>102</v>
+      </c>
+      <c r="D41" s="3" t="s">
+        <v>101</v>
+      </c>
+      <c r="E41" s="3" t="s">
+        <v>99</v>
+      </c>
+      <c r="F41" s="3" t="s">
+        <v>100</v>
+      </c>
+      <c r="G41" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="H41" s="3" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="42" spans="1:9" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="A42" s="3" t="s">
+        <v>131</v>
+      </c>
+      <c r="B42" s="3" t="s">
+        <v>67</v>
+      </c>
+      <c r="C42" s="3" t="s">
         <v>132</v>
       </c>
-      <c r="F40" s="3" t="s">
-        <v>131</v>
-      </c>
-      <c r="G40" s="3" t="s">
-        <v>6</v>
-      </c>
-      <c r="H40" s="3" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="41" spans="1:9" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="A41" s="3" t="s">
-        <v>70</v>
-      </c>
-      <c r="B41" s="3" t="s">
-        <v>69</v>
-      </c>
-      <c r="C41" s="3" t="s">
+      <c r="D42" s="3" t="s">
         <v>133</v>
       </c>
-      <c r="D41" s="3" t="s">
-        <v>134</v>
-      </c>
-      <c r="E41" s="5" t="s">
-        <v>71</v>
-      </c>
-      <c r="F41" s="5" t="s">
-        <v>72</v>
-      </c>
-      <c r="G41" s="3" t="s">
-        <v>6</v>
-      </c>
-      <c r="H41" s="3" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="42" spans="1:9" ht="15" x14ac:dyDescent="0.25">
-      <c r="A42" s="4" t="s">
-        <v>135</v>
-      </c>
-      <c r="B42" s="3" t="s">
-        <v>69</v>
-      </c>
-      <c r="C42" s="3" t="s">
-        <v>104</v>
-      </c>
-      <c r="D42" s="3" t="s">
-        <v>103</v>
-      </c>
       <c r="E42" s="3" t="s">
-        <v>101</v>
+        <v>148</v>
       </c>
       <c r="F42" s="3" t="s">
-        <v>102</v>
+        <v>149</v>
       </c>
       <c r="G42" s="3" t="s">
         <v>6</v>
@@ -2100,22 +2085,22 @@
     </row>
     <row r="43" spans="1:9" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A43" s="3" t="s">
-        <v>136</v>
+        <v>134</v>
       </c>
       <c r="B43" s="3" t="s">
+        <v>67</v>
+      </c>
+      <c r="C43" s="5" t="s">
         <v>69</v>
       </c>
-      <c r="C43" s="3" t="s">
-        <v>137</v>
-      </c>
-      <c r="D43" s="3" t="s">
-        <v>138</v>
+      <c r="D43" s="5" t="s">
+        <v>70</v>
       </c>
       <c r="E43" s="3" t="s">
-        <v>153</v>
+        <v>34</v>
       </c>
       <c r="F43" s="3" t="s">
-        <v>154</v>
+        <v>35</v>
       </c>
       <c r="G43" s="3" t="s">
         <v>6</v>
@@ -2126,22 +2111,22 @@
     </row>
     <row r="44" spans="1:9" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A44" s="3" t="s">
-        <v>139</v>
+        <v>71</v>
       </c>
       <c r="B44" s="3" t="s">
-        <v>69</v>
-      </c>
-      <c r="C44" s="5" t="s">
-        <v>71</v>
-      </c>
-      <c r="D44" s="5" t="s">
+        <v>67</v>
+      </c>
+      <c r="C44" s="3" t="s">
         <v>72</v>
       </c>
+      <c r="D44" s="3" t="s">
+        <v>73</v>
+      </c>
       <c r="E44" s="3" t="s">
-        <v>34</v>
+        <v>72</v>
       </c>
       <c r="F44" s="3" t="s">
-        <v>35</v>
+        <v>73</v>
       </c>
       <c r="G44" s="3" t="s">
         <v>6</v>
@@ -2150,24 +2135,24 @@
         <v>6</v>
       </c>
     </row>
-    <row r="45" spans="1:9" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="45" spans="1:9" s="6" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A45" s="3" t="s">
-        <v>73</v>
+        <v>197</v>
       </c>
       <c r="B45" s="3" t="s">
-        <v>69</v>
+        <v>75</v>
       </c>
       <c r="C45" s="3" t="s">
-        <v>74</v>
+        <v>179</v>
       </c>
       <c r="D45" s="3" t="s">
-        <v>75</v>
+        <v>180</v>
       </c>
       <c r="E45" s="3" t="s">
-        <v>74</v>
+        <v>173</v>
       </c>
       <c r="F45" s="3" t="s">
-        <v>75</v>
+        <v>174</v>
       </c>
       <c r="G45" s="3" t="s">
         <v>6</v>
@@ -2178,22 +2163,22 @@
     </row>
     <row r="46" spans="1:9" s="6" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A46" s="3" t="s">
-        <v>203</v>
+        <v>74</v>
       </c>
       <c r="B46" s="3" t="s">
+        <v>75</v>
+      </c>
+      <c r="C46" s="3" t="s">
+        <v>76</v>
+      </c>
+      <c r="D46" s="3" t="s">
         <v>77</v>
       </c>
-      <c r="C46" s="3" t="s">
-        <v>184</v>
-      </c>
-      <c r="D46" s="3" t="s">
-        <v>185</v>
-      </c>
       <c r="E46" s="3" t="s">
-        <v>178</v>
+        <v>76</v>
       </c>
       <c r="F46" s="3" t="s">
-        <v>179</v>
+        <v>77</v>
       </c>
       <c r="G46" s="3" t="s">
         <v>6</v>
@@ -2204,48 +2189,48 @@
     </row>
     <row r="47" spans="1:9" s="6" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A47" s="3" t="s">
+        <v>74</v>
+      </c>
+      <c r="B47" s="3" t="s">
+        <v>75</v>
+      </c>
+      <c r="C47" s="3" t="s">
         <v>76</v>
       </c>
-      <c r="B47" s="3" t="s">
-        <v>77</v>
-      </c>
-      <c r="C47" s="3" t="s">
+      <c r="D47" s="3" t="s">
         <v>78</v>
       </c>
-      <c r="D47" s="3" t="s">
+      <c r="E47" s="3" t="s">
+        <v>76</v>
+      </c>
+      <c r="F47" s="3" t="s">
+        <v>78</v>
+      </c>
+      <c r="G47" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="H47" s="3" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="48" spans="1:9" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="A48" s="3" t="s">
         <v>79</v>
       </c>
-      <c r="E47" s="3" t="s">
-        <v>78</v>
-      </c>
-      <c r="F47" s="3" t="s">
-        <v>79</v>
-      </c>
-      <c r="G47" s="3" t="s">
-        <v>6</v>
-      </c>
-      <c r="H47" s="3" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="48" spans="1:9" s="6" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="A48" s="3" t="s">
-        <v>76</v>
-      </c>
       <c r="B48" s="3" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="C48" s="3" t="s">
-        <v>78</v>
+        <v>170</v>
       </c>
       <c r="D48" s="3" t="s">
+        <v>171</v>
+      </c>
+      <c r="E48" s="3" t="s">
         <v>80</v>
       </c>
-      <c r="E48" s="3" t="s">
-        <v>78</v>
-      </c>
       <c r="F48" s="3" t="s">
-        <v>80</v>
+        <v>81</v>
       </c>
       <c r="G48" s="3" t="s">
         <v>6</v>
@@ -2254,24 +2239,24 @@
         <v>6</v>
       </c>
     </row>
-    <row r="49" spans="1:8" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="49" spans="1:8" s="6" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A49" s="3" t="s">
-        <v>81</v>
+        <v>172</v>
       </c>
       <c r="B49" s="3" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="C49" s="3" t="s">
-        <v>175</v>
+        <v>173</v>
       </c>
       <c r="D49" s="3" t="s">
-        <v>176</v>
+        <v>174</v>
       </c>
       <c r="E49" s="3" t="s">
-        <v>82</v>
+        <v>173</v>
       </c>
       <c r="F49" s="3" t="s">
-        <v>83</v>
+        <v>174</v>
       </c>
       <c r="G49" s="3" t="s">
         <v>6</v>
@@ -2280,24 +2265,24 @@
         <v>6</v>
       </c>
     </row>
-    <row r="50" spans="1:8" s="6" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="50" spans="1:8" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A50" s="3" t="s">
-        <v>177</v>
+        <v>135</v>
       </c>
       <c r="B50" s="3" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="C50" s="3" t="s">
-        <v>178</v>
+        <v>85</v>
       </c>
       <c r="D50" s="3" t="s">
-        <v>179</v>
+        <v>86</v>
       </c>
       <c r="E50" s="3" t="s">
-        <v>178</v>
+        <v>87</v>
       </c>
       <c r="F50" s="3" t="s">
-        <v>179</v>
+        <v>88</v>
       </c>
       <c r="G50" s="3" t="s">
         <v>6</v>
@@ -2308,22 +2293,22 @@
     </row>
     <row r="51" spans="1:8" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A51" s="3" t="s">
-        <v>140</v>
+        <v>82</v>
       </c>
       <c r="B51" s="3" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="C51" s="3" t="s">
-        <v>87</v>
+        <v>83</v>
       </c>
       <c r="D51" s="3" t="s">
-        <v>88</v>
+        <v>84</v>
       </c>
       <c r="E51" s="3" t="s">
-        <v>89</v>
+        <v>83</v>
       </c>
       <c r="F51" s="3" t="s">
-        <v>90</v>
+        <v>84</v>
       </c>
       <c r="G51" s="3" t="s">
         <v>6</v>
@@ -2334,22 +2319,22 @@
     </row>
     <row r="52" spans="1:8" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A52" s="3" t="s">
-        <v>84</v>
+        <v>136</v>
       </c>
       <c r="B52" s="3" t="s">
-        <v>77</v>
-      </c>
-      <c r="C52" s="3" t="s">
-        <v>85</v>
-      </c>
-      <c r="D52" s="3" t="s">
-        <v>86</v>
+        <v>75</v>
+      </c>
+      <c r="C52" s="6" t="s">
+        <v>142</v>
+      </c>
+      <c r="D52" s="6" t="s">
+        <v>143</v>
       </c>
       <c r="E52" s="3" t="s">
-        <v>85</v>
+        <v>137</v>
       </c>
       <c r="F52" s="3" t="s">
-        <v>86</v>
+        <v>138</v>
       </c>
       <c r="G52" s="3" t="s">
         <v>6</v>
@@ -2360,21 +2345,21 @@
     </row>
     <row r="53" spans="1:8" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A53" s="3" t="s">
+        <v>139</v>
+      </c>
+      <c r="B53" s="3" t="s">
+        <v>75</v>
+      </c>
+      <c r="C53" t="s">
+        <v>140</v>
+      </c>
+      <c r="D53" t="s">
         <v>141</v>
       </c>
-      <c r="B53" s="3" t="s">
-        <v>77</v>
-      </c>
-      <c r="C53" s="6" t="s">
-        <v>147</v>
-      </c>
-      <c r="D53" s="6" t="s">
-        <v>148</v>
-      </c>
-      <c r="E53" s="3" t="s">
+      <c r="E53" s="6" t="s">
         <v>142</v>
       </c>
-      <c r="F53" s="3" t="s">
+      <c r="F53" s="6" t="s">
         <v>143</v>
       </c>
       <c r="G53" s="3" t="s">
@@ -2386,22 +2371,22 @@
     </row>
     <row r="54" spans="1:8" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A54" s="3" t="s">
-        <v>144</v>
+        <v>150</v>
       </c>
       <c r="B54" s="3" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="C54" t="s">
-        <v>145</v>
+        <v>151</v>
       </c>
       <c r="D54" t="s">
-        <v>146</v>
+        <v>152</v>
       </c>
       <c r="E54" s="6" t="s">
-        <v>147</v>
+        <v>151</v>
       </c>
       <c r="F54" s="6" t="s">
-        <v>148</v>
+        <v>152</v>
       </c>
       <c r="G54" s="3" t="s">
         <v>6</v>
@@ -2410,34 +2395,18 @@
         <v>6</v>
       </c>
     </row>
-    <row r="55" spans="1:8" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="A55" s="3" t="s">
-        <v>155</v>
-      </c>
-      <c r="B55" s="3" t="s">
-        <v>77</v>
-      </c>
-      <c r="C55" t="s">
-        <v>156</v>
-      </c>
-      <c r="D55" t="s">
-        <v>157</v>
-      </c>
-      <c r="E55" s="6" t="s">
-        <v>156</v>
-      </c>
-      <c r="F55" s="6" t="s">
-        <v>157</v>
-      </c>
-      <c r="G55" s="3" t="s">
-        <v>6</v>
-      </c>
-      <c r="H55" s="3" t="s">
-        <v>6</v>
-      </c>
-    </row>
+    <row r="55" spans="1:8" ht="12.75" x14ac:dyDescent="0.2"/>
     <row r="56" spans="1:8" ht="12.75" x14ac:dyDescent="0.2"/>
-    <row r="57" spans="1:8" ht="12.75" x14ac:dyDescent="0.2"/>
+    <row r="57" spans="1:8" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="A57" s="3"/>
+      <c r="B57" s="3"/>
+      <c r="C57" s="3"/>
+      <c r="D57" s="3"/>
+      <c r="E57" s="3"/>
+      <c r="F57" s="3"/>
+      <c r="G57" s="3"/>
+      <c r="H57" s="3"/>
+    </row>
     <row r="58" spans="1:8" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A58" s="3"/>
       <c r="B58" s="3"/>
@@ -2448,17 +2417,17 @@
       <c r="G58" s="3"/>
       <c r="H58" s="3"/>
     </row>
-    <row r="59" spans="1:8" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="A59" s="3"/>
-      <c r="B59" s="3"/>
-      <c r="C59" s="3"/>
-      <c r="D59" s="3"/>
-      <c r="E59" s="3"/>
-      <c r="F59" s="3"/>
-      <c r="G59" s="3"/>
-      <c r="H59" s="3"/>
-    </row>
-    <row r="60" spans="1:8" ht="12.75" x14ac:dyDescent="0.2"/>
+    <row r="59" spans="1:8" ht="12.75" x14ac:dyDescent="0.2"/>
+    <row r="60" spans="1:8" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="A60" s="3"/>
+      <c r="B60" s="3"/>
+      <c r="C60" s="3"/>
+      <c r="D60" s="3"/>
+      <c r="E60" s="3"/>
+      <c r="F60" s="3"/>
+      <c r="G60" s="3"/>
+      <c r="H60" s="3"/>
+    </row>
     <row r="61" spans="1:8" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A61" s="3"/>
       <c r="B61" s="3"/>
@@ -2469,21 +2438,21 @@
       <c r="G61" s="3"/>
       <c r="H61" s="3"/>
     </row>
-    <row r="62" spans="1:8" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="62" spans="1:8" s="6" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A62" s="3"/>
       <c r="B62" s="3"/>
-      <c r="C62" s="3"/>
-      <c r="D62" s="3"/>
+      <c r="C62" s="5"/>
+      <c r="D62" s="5"/>
       <c r="E62" s="3"/>
       <c r="F62" s="3"/>
       <c r="G62" s="3"/>
       <c r="H62" s="3"/>
     </row>
-    <row r="63" spans="1:8" s="6" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="63" spans="1:8" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A63" s="3"/>
       <c r="B63" s="3"/>
-      <c r="C63" s="5"/>
-      <c r="D63" s="5"/>
+      <c r="C63" s="3"/>
+      <c r="D63" s="3"/>
       <c r="E63" s="3"/>
       <c r="F63" s="3"/>
       <c r="G63" s="3"/>
@@ -2499,45 +2468,38 @@
       <c r="G64" s="3"/>
       <c r="H64" s="3"/>
     </row>
-    <row r="65" spans="1:8" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="A65" s="3"/>
-      <c r="B65" s="3"/>
-      <c r="C65" s="3"/>
-      <c r="D65" s="3"/>
-      <c r="E65" s="3"/>
-      <c r="F65" s="3"/>
-      <c r="G65" s="3"/>
-      <c r="H65" s="3"/>
-    </row>
-    <row r="66" spans="1:8" ht="12.75" x14ac:dyDescent="0.2"/>
-    <row r="67" spans="1:8" ht="12.75" x14ac:dyDescent="0.2"/>
-    <row r="68" spans="1:8" ht="12.75" x14ac:dyDescent="0.2"/>
-    <row r="69" spans="1:8" ht="12.75" x14ac:dyDescent="0.2"/>
-    <row r="70" spans="1:8" ht="12.75" x14ac:dyDescent="0.2"/>
-    <row r="71" spans="1:8" ht="12.75" x14ac:dyDescent="0.2"/>
-    <row r="72" spans="1:8" ht="12.75" x14ac:dyDescent="0.2"/>
-    <row r="73" spans="1:8" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="65" spans="2:2" ht="12.75" x14ac:dyDescent="0.2"/>
+    <row r="66" spans="2:2" ht="12.75" x14ac:dyDescent="0.2"/>
+    <row r="67" spans="2:2" ht="12.75" x14ac:dyDescent="0.2"/>
+    <row r="68" spans="2:2" ht="12.75" x14ac:dyDescent="0.2"/>
+    <row r="69" spans="2:2" ht="12.75" x14ac:dyDescent="0.2"/>
+    <row r="70" spans="2:2" ht="12.75" x14ac:dyDescent="0.2"/>
+    <row r="71" spans="2:2" ht="12.75" x14ac:dyDescent="0.2"/>
+    <row r="72" spans="2:2" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="B72" s="7"/>
+    </row>
+    <row r="73" spans="2:2" ht="12.75" x14ac:dyDescent="0.2">
       <c r="B73" s="7"/>
     </row>
-    <row r="74" spans="1:8" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="74" spans="2:2" ht="12.75" x14ac:dyDescent="0.2">
       <c r="B74" s="7"/>
     </row>
-    <row r="75" spans="1:8" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="75" spans="2:2" ht="12.75" x14ac:dyDescent="0.2">
       <c r="B75" s="7"/>
     </row>
-    <row r="76" spans="1:8" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="76" spans="2:2" ht="12.75" x14ac:dyDescent="0.2">
       <c r="B76" s="7"/>
     </row>
-    <row r="77" spans="1:8" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="77" spans="2:2" ht="12.75" x14ac:dyDescent="0.2">
       <c r="B77" s="7"/>
     </row>
-    <row r="78" spans="1:8" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="78" spans="2:2" ht="12.75" x14ac:dyDescent="0.2">
       <c r="B78" s="7"/>
     </row>
-    <row r="79" spans="1:8" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="79" spans="2:2" ht="12.75" x14ac:dyDescent="0.2">
       <c r="B79" s="7"/>
     </row>
-    <row r="80" spans="1:8" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="80" spans="2:2" ht="12.75" x14ac:dyDescent="0.2">
       <c r="B80" s="7"/>
     </row>
     <row r="81" spans="2:2" ht="12.75" x14ac:dyDescent="0.2">
@@ -5341,9 +5303,6 @@
     </row>
     <row r="1014" spans="2:2" ht="12.75" x14ac:dyDescent="0.2">
       <c r="B1014" s="7"/>
-    </row>
-    <row r="1015" spans="2:2" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="B1015" s="7"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -5355,7 +5314,7 @@
           <x14:formula1>
             <xm:f>Class!$A$2:$A$9</xm:f>
           </x14:formula1>
-          <xm:sqref>B58:B59 B73:B1015 B61:B65 B4:B55</xm:sqref>
+          <xm:sqref>B57:B58 B72:B1014 B60:B64 B4:B54</xm:sqref>
         </x14:dataValidation>
       </x14:dataValidations>
     </ext>
@@ -5376,7 +5335,7 @@
   <sheetData>
     <row r="1" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A1" s="8" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
     </row>
     <row r="2" spans="1:1" x14ac:dyDescent="0.2">
@@ -5401,22 +5360,22 @@
     </row>
     <row r="6" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A6" s="3" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
     </row>
     <row r="7" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A7" s="3" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
     </row>
     <row r="8" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A8" s="3" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
     </row>
     <row r="9" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A9" s="3" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
     </row>
   </sheetData>

</xml_diff>